<commit_message>
Homework 3 question 5
</commit_message>
<xml_diff>
--- a/2020 Summer/CSE 5321 Software Testing/Homework 3/Homework-03.xlsx
+++ b/2020 Summer/CSE 5321 Software Testing/Homework 3/Homework-03.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gaura\Documents\Academic\UTA\2020 Summer\CSE 5321 Software Testing\Homework 3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76CF7693-7D60-4CC2-B26B-C986E09A5096}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{310D1D8D-8D13-4AC1-A348-E4544A415127}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="4" xr2:uid="{CA2C47C1-9B3A-4639-99C1-0BD544F6496B}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="6" xr2:uid="{CA2C47C1-9B3A-4639-99C1-0BD544F6496B}"/>
   </bookViews>
   <sheets>
     <sheet name="1.1" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="2.2" sheetId="4" r:id="rId4"/>
     <sheet name="3.1" sheetId="5" r:id="rId5"/>
     <sheet name="4" sheetId="6" r:id="rId6"/>
+    <sheet name="5" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="376" uniqueCount="224">
   <si>
     <t>Test Case Number</t>
   </si>
@@ -639,6 +640,215 @@
   <si>
     <t>tc6</t>
   </si>
+  <si>
+    <t>Output</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
+    <t>-2.00 : -1.01</t>
+  </si>
+  <si>
+    <t>-1.00 : -0.01</t>
+  </si>
+  <si>
+    <t>0.00 : 2.00</t>
+  </si>
+  <si>
+    <t>2.01 : 6.00</t>
+  </si>
+  <si>
+    <t>6.01 : 8.00</t>
+  </si>
+  <si>
+    <t>8.01 : 9.00</t>
+  </si>
+  <si>
+    <t>9.01 : 10.00</t>
+  </si>
+  <si>
+    <t>-1.01</t>
+  </si>
+  <si>
+    <t>8-9-27</t>
+  </si>
+  <si>
+    <t>8-11-12-27</t>
+  </si>
+  <si>
+    <t>8-11-14-15-27</t>
+  </si>
+  <si>
+    <t>8-11-14-17-18-27</t>
+  </si>
+  <si>
+    <t>8-11-14-17-20-21-27</t>
+  </si>
+  <si>
+    <t>8-11-14-17-20-23-24-27</t>
+  </si>
+  <si>
+    <t>8-11-14-17-20-23-26-27</t>
+  </si>
+  <si>
+    <t>-0.01</t>
+  </si>
+  <si>
+    <t>abcdef</t>
+  </si>
+  <si>
+    <t>TTTTTT</t>
+  </si>
+  <si>
+    <r>
+      <t>T</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>F</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>TTTT</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>F</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>TTTTT</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>TT</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>F</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>TTT</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>TTT</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>F</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>TT</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>TTTT</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>F</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>T</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>TTTTT</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>F</t>
+    </r>
+  </si>
+  <si>
+    <t>if (x &lt; -1.00 &amp;&amp; x &lt; 0.0 &amp;&amp; x &lt;= 2.0 &amp;&amp; x &lt;= 6.0 &amp;&amp; x &lt;= 8.0 &amp;&amp; x &lt;= 9.0)</t>
+  </si>
 </sst>
 </file>
 
@@ -650,7 +860,7 @@
     <numFmt numFmtId="165" formatCode="0.0"/>
     <numFmt numFmtId="166" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -758,8 +968,48 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF7030A0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="9" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="7" tint="0.39997558519241921"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="5"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -787,6 +1037,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -915,7 +1171,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="98">
+  <cellXfs count="117">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1049,6 +1305,30 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1057,24 +1337,6 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1091,6 +1353,9 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1099,44 +1364,59 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1144,28 +1424,57 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1375,6 +1684,54 @@
         <a:xfrm>
           <a:off x="6659881" y="0"/>
           <a:ext cx="2903219" cy="4151376"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>106681</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>167640</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>617220</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>112776</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FF5C17D7-F435-4601-A8B4-2F98EB36F14A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:srcRect r="56795"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3764281" y="731520"/>
+          <a:ext cx="2689859" cy="4151376"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1710,23 +2067,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A1" s="59" t="s">
+      <c r="A1" s="67" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="60" t="s">
+      <c r="C1" s="68" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="60"/>
-      <c r="E1" s="63" t="s">
+      <c r="D1" s="68"/>
+      <c r="E1" s="61" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="64"/>
+      <c r="F1" s="62"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" s="59"/>
+      <c r="A2" s="67"/>
       <c r="B2" s="19" t="s">
         <v>2</v>
       </c>
@@ -1736,8 +2093,8 @@
       <c r="D2" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="65"/>
-      <c r="F2" s="66"/>
+      <c r="E2" s="63"/>
+      <c r="F2" s="64"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="22">
@@ -1752,10 +2109,10 @@
       <c r="D3" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="57" t="s">
+      <c r="E3" s="65" t="s">
         <v>16</v>
       </c>
-      <c r="F3" s="58"/>
+      <c r="F3" s="66"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="22">
@@ -1770,10 +2127,10 @@
       <c r="D4" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="E4" s="57" t="s">
+      <c r="E4" s="65" t="s">
         <v>17</v>
       </c>
-      <c r="F4" s="58"/>
+      <c r="F4" s="66"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="22">
@@ -1788,10 +2145,10 @@
       <c r="D5" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="E5" s="57" t="s">
+      <c r="E5" s="65" t="s">
         <v>18</v>
       </c>
-      <c r="F5" s="58"/>
+      <c r="F5" s="66"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="22">
@@ -1806,10 +2163,10 @@
       <c r="D6" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="E6" s="57" t="s">
+      <c r="E6" s="65" t="s">
         <v>19</v>
       </c>
-      <c r="F6" s="58"/>
+      <c r="F6" s="66"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="22">
@@ -1824,10 +2181,10 @@
       <c r="D7" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="E7" s="57" t="s">
+      <c r="E7" s="65" t="s">
         <v>20</v>
       </c>
-      <c r="F7" s="58"/>
+      <c r="F7" s="66"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="22">
@@ -1842,10 +2199,10 @@
       <c r="D8" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="E8" s="57" t="s">
+      <c r="E8" s="65" t="s">
         <v>21</v>
       </c>
-      <c r="F8" s="58"/>
+      <c r="F8" s="66"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="22">
@@ -1860,10 +2217,10 @@
       <c r="D9" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="E9" s="57" t="s">
+      <c r="E9" s="65" t="s">
         <v>22</v>
       </c>
-      <c r="F9" s="58"/>
+      <c r="F9" s="66"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="22">
@@ -1878,10 +2235,10 @@
       <c r="D10" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="E10" s="57" t="s">
+      <c r="E10" s="65" t="s">
         <v>23</v>
       </c>
-      <c r="F10" s="58"/>
+      <c r="F10" s="66"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="23">
@@ -1896,10 +2253,10 @@
       <c r="D11" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="E11" s="61" t="s">
+      <c r="E11" s="59" t="s">
         <v>24</v>
       </c>
-      <c r="F11" s="62"/>
+      <c r="F11" s="60"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="23">
@@ -1914,10 +2271,10 @@
       <c r="D12" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="E12" s="61" t="s">
+      <c r="E12" s="59" t="s">
         <v>24</v>
       </c>
-      <c r="F12" s="62"/>
+      <c r="F12" s="60"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="23">
@@ -1932,10 +2289,10 @@
       <c r="D13" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="E13" s="61" t="s">
+      <c r="E13" s="59" t="s">
         <v>24</v>
       </c>
-      <c r="F13" s="62"/>
+      <c r="F13" s="60"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="23">
@@ -1950,10 +2307,10 @@
       <c r="D14" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="E14" s="61" t="s">
+      <c r="E14" s="59" t="s">
         <v>24</v>
       </c>
-      <c r="F14" s="62"/>
+      <c r="F14" s="60"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="23">
@@ -1968,10 +2325,10 @@
       <c r="D15" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="E15" s="61" t="s">
+      <c r="E15" s="59" t="s">
         <v>24</v>
       </c>
-      <c r="F15" s="62"/>
+      <c r="F15" s="60"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" s="23">
@@ -1986,10 +2343,10 @@
       <c r="D16" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="E16" s="61" t="s">
+      <c r="E16" s="59" t="s">
         <v>24</v>
       </c>
-      <c r="F16" s="62"/>
+      <c r="F16" s="60"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" s="23">
@@ -2004,10 +2361,10 @@
       <c r="D17" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="E17" s="61" t="s">
+      <c r="E17" s="59" t="s">
         <v>24</v>
       </c>
-      <c r="F17" s="62"/>
+      <c r="F17" s="60"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" s="21"/>
@@ -2068,6 +2425,9 @@
     <sortCondition descending="1" ref="B11"/>
   </sortState>
   <mergeCells count="18">
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="E15:F15"/>
     <mergeCell ref="E16:F16"/>
     <mergeCell ref="E17:F17"/>
     <mergeCell ref="E1:F2"/>
@@ -2083,9 +2443,6 @@
     <mergeCell ref="E6:F6"/>
     <mergeCell ref="E7:F7"/>
     <mergeCell ref="E8:F8"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="E15:F15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
@@ -2113,44 +2470,44 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A1" s="70" t="s">
+      <c r="A1" s="72" t="s">
         <v>40</v>
       </c>
-      <c r="B1" s="67" t="s">
+      <c r="B1" s="69" t="s">
         <v>32</v>
       </c>
-      <c r="C1" s="67" t="s">
+      <c r="C1" s="69" t="s">
         <v>33</v>
       </c>
-      <c r="D1" s="67" t="s">
+      <c r="D1" s="69" t="s">
         <v>34</v>
       </c>
-      <c r="E1" s="67" t="s">
+      <c r="E1" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="F1" s="67" t="s">
+      <c r="F1" s="69" t="s">
         <v>36</v>
       </c>
-      <c r="G1" s="67" t="s">
+      <c r="G1" s="69" t="s">
         <v>37</v>
       </c>
-      <c r="H1" s="67" t="s">
+      <c r="H1" s="69" t="s">
         <v>38</v>
       </c>
-      <c r="I1" s="67" t="s">
+      <c r="I1" s="69" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A2" s="71"/>
-      <c r="B2" s="68"/>
-      <c r="C2" s="68"/>
-      <c r="D2" s="68"/>
-      <c r="E2" s="68"/>
-      <c r="F2" s="68"/>
-      <c r="G2" s="68"/>
-      <c r="H2" s="68"/>
-      <c r="I2" s="68"/>
+      <c r="A2" s="73"/>
+      <c r="B2" s="70"/>
+      <c r="C2" s="70"/>
+      <c r="D2" s="70"/>
+      <c r="E2" s="70"/>
+      <c r="F2" s="70"/>
+      <c r="G2" s="70"/>
+      <c r="H2" s="70"/>
+      <c r="I2" s="70"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
@@ -2273,17 +2630,17 @@
       </c>
     </row>
     <row r="11" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="69" t="s">
+      <c r="A11" s="71" t="s">
         <v>43</v>
       </c>
-      <c r="B11" s="69"/>
-      <c r="C11" s="69"/>
-      <c r="D11" s="69"/>
-      <c r="E11" s="69"/>
-      <c r="F11" s="69"/>
-      <c r="G11" s="69"/>
-      <c r="H11" s="69"/>
-      <c r="I11" s="69"/>
+      <c r="B11" s="71"/>
+      <c r="C11" s="71"/>
+      <c r="D11" s="71"/>
+      <c r="E11" s="71"/>
+      <c r="F11" s="71"/>
+      <c r="G11" s="71"/>
+      <c r="H11" s="71"/>
+      <c r="I11" s="71"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
@@ -2383,57 +2740,57 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="16" customFormat="1" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="75" t="s">
+      <c r="A1" s="74" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="72" t="s">
+      <c r="C1" s="75" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="72"/>
-      <c r="E1" s="72"/>
-      <c r="F1" s="72"/>
-      <c r="G1" s="72"/>
-      <c r="H1" s="72" t="s">
+      <c r="D1" s="75"/>
+      <c r="E1" s="75"/>
+      <c r="F1" s="75"/>
+      <c r="G1" s="75"/>
+      <c r="H1" s="75" t="s">
         <v>56</v>
       </c>
-      <c r="I1" s="72"/>
+      <c r="I1" s="75"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A2" s="75"/>
-      <c r="B2" s="73" t="s">
+      <c r="A2" s="74"/>
+      <c r="B2" s="76" t="s">
         <v>50</v>
       </c>
-      <c r="C2" s="72" t="s">
+      <c r="C2" s="75" t="s">
         <v>51</v>
       </c>
-      <c r="D2" s="72" t="s">
+      <c r="D2" s="75" t="s">
         <v>52</v>
       </c>
-      <c r="E2" s="75" t="s">
+      <c r="E2" s="74" t="s">
         <v>53</v>
       </c>
-      <c r="F2" s="75" t="s">
+      <c r="F2" s="74" t="s">
         <v>54</v>
       </c>
-      <c r="G2" s="72" t="s">
+      <c r="G2" s="75" t="s">
         <v>55</v>
       </c>
-      <c r="H2" s="72"/>
-      <c r="I2" s="72"/>
+      <c r="H2" s="75"/>
+      <c r="I2" s="75"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A3" s="75"/>
-      <c r="B3" s="73"/>
-      <c r="C3" s="72"/>
-      <c r="D3" s="72"/>
-      <c r="E3" s="75"/>
-      <c r="F3" s="75"/>
-      <c r="G3" s="72"/>
-      <c r="H3" s="72"/>
-      <c r="I3" s="72"/>
+      <c r="A3" s="74"/>
+      <c r="B3" s="76"/>
+      <c r="C3" s="75"/>
+      <c r="D3" s="75"/>
+      <c r="E3" s="74"/>
+      <c r="F3" s="74"/>
+      <c r="G3" s="75"/>
+      <c r="H3" s="75"/>
+      <c r="I3" s="75"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="7">
@@ -2457,10 +2814,10 @@
       <c r="G4" s="17" t="b">
         <v>1</v>
       </c>
-      <c r="H4" s="76" t="s">
+      <c r="H4" s="78" t="s">
         <v>68</v>
       </c>
-      <c r="I4" s="76"/>
+      <c r="I4" s="78"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="7">
@@ -2484,10 +2841,10 @@
       <c r="G5" s="12" t="b">
         <v>0</v>
       </c>
-      <c r="H5" s="76" t="s">
+      <c r="H5" s="78" t="s">
         <v>69</v>
       </c>
-      <c r="I5" s="76"/>
+      <c r="I5" s="78"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="7">
@@ -2511,10 +2868,10 @@
       <c r="G6" s="7" t="b">
         <v>1</v>
       </c>
-      <c r="H6" s="76" t="s">
+      <c r="H6" s="78" t="s">
         <v>70</v>
       </c>
-      <c r="I6" s="76"/>
+      <c r="I6" s="78"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="7">
@@ -2538,10 +2895,10 @@
       <c r="G7" s="7" t="b">
         <v>1</v>
       </c>
-      <c r="H7" s="76" t="s">
+      <c r="H7" s="78" t="s">
         <v>71</v>
       </c>
-      <c r="I7" s="76"/>
+      <c r="I7" s="78"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="7">
@@ -2565,10 +2922,10 @@
       <c r="G8" s="7" t="b">
         <v>1</v>
       </c>
-      <c r="H8" s="76" t="s">
+      <c r="H8" s="78" t="s">
         <v>72</v>
       </c>
-      <c r="I8" s="76"/>
+      <c r="I8" s="78"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="7">
@@ -2592,10 +2949,10 @@
       <c r="G9" s="7" t="b">
         <v>1</v>
       </c>
-      <c r="H9" s="76" t="s">
+      <c r="H9" s="78" t="s">
         <v>73</v>
       </c>
-      <c r="I9" s="76"/>
+      <c r="I9" s="78"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="7">
@@ -2619,10 +2976,10 @@
       <c r="G10" s="7" t="b">
         <v>1</v>
       </c>
-      <c r="H10" s="76" t="s">
+      <c r="H10" s="78" t="s">
         <v>74</v>
       </c>
-      <c r="I10" s="76"/>
+      <c r="I10" s="78"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="11">
@@ -2646,10 +3003,10 @@
       <c r="G11" s="14" t="b">
         <v>0</v>
       </c>
-      <c r="H11" s="74" t="s">
+      <c r="H11" s="77" t="s">
         <v>24</v>
       </c>
-      <c r="I11" s="74"/>
+      <c r="I11" s="77"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="11">
@@ -2673,10 +3030,10 @@
       <c r="G12" s="11" t="b">
         <v>1</v>
       </c>
-      <c r="H12" s="74" t="s">
+      <c r="H12" s="77" t="s">
         <v>24</v>
       </c>
-      <c r="I12" s="74"/>
+      <c r="I12" s="77"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="11">
@@ -2700,10 +3057,10 @@
       <c r="G13" s="11" t="b">
         <v>1</v>
       </c>
-      <c r="H13" s="74" t="s">
+      <c r="H13" s="77" t="s">
         <v>24</v>
       </c>
-      <c r="I13" s="74"/>
+      <c r="I13" s="77"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" s="11">
@@ -2727,10 +3084,10 @@
       <c r="G14" s="11" t="b">
         <v>1</v>
       </c>
-      <c r="H14" s="74" t="s">
+      <c r="H14" s="77" t="s">
         <v>24</v>
       </c>
-      <c r="I14" s="74"/>
+      <c r="I14" s="77"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" s="11">
@@ -2754,10 +3111,10 @@
       <c r="G15" s="11" t="b">
         <v>1</v>
       </c>
-      <c r="H15" s="74" t="s">
+      <c r="H15" s="77" t="s">
         <v>24</v>
       </c>
-      <c r="I15" s="74"/>
+      <c r="I15" s="77"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" s="11">
@@ -2781,10 +3138,10 @@
       <c r="G16" s="11" t="b">
         <v>1</v>
       </c>
-      <c r="H16" s="74" t="s">
+      <c r="H16" s="77" t="s">
         <v>24</v>
       </c>
-      <c r="I16" s="74"/>
+      <c r="I16" s="77"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" s="13" t="s">
@@ -2823,12 +3180,6 @@
     </row>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="A1:A3"/>
-    <mergeCell ref="C1:G1"/>
-    <mergeCell ref="G2:G3"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="C2:C3"/>
     <mergeCell ref="H1:I3"/>
     <mergeCell ref="B2:B3"/>
     <mergeCell ref="H16:I16"/>
@@ -2845,6 +3196,12 @@
     <mergeCell ref="H9:I9"/>
     <mergeCell ref="H8:I8"/>
     <mergeCell ref="H7:I7"/>
+    <mergeCell ref="A1:A3"/>
+    <mergeCell ref="C1:G1"/>
+    <mergeCell ref="G2:G3"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="C2:C3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
@@ -2866,40 +3223,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="70" t="s">
+      <c r="A1" s="72" t="s">
         <v>57</v>
       </c>
-      <c r="B1" s="67" t="s">
+      <c r="B1" s="69" t="s">
         <v>32</v>
       </c>
-      <c r="C1" s="67" t="s">
+      <c r="C1" s="69" t="s">
         <v>33</v>
       </c>
-      <c r="D1" s="67" t="s">
+      <c r="D1" s="69" t="s">
         <v>34</v>
       </c>
-      <c r="E1" s="67" t="s">
+      <c r="E1" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="F1" s="67" t="s">
+      <c r="F1" s="69" t="s">
         <v>36</v>
       </c>
-      <c r="G1" s="67" t="s">
+      <c r="G1" s="69" t="s">
         <v>37</v>
       </c>
-      <c r="H1" s="67" t="s">
+      <c r="H1" s="69" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2" s="71"/>
-      <c r="B2" s="68"/>
-      <c r="C2" s="68"/>
-      <c r="D2" s="68"/>
-      <c r="E2" s="68"/>
-      <c r="F2" s="68"/>
-      <c r="G2" s="68"/>
-      <c r="H2" s="68"/>
+      <c r="A2" s="73"/>
+      <c r="B2" s="70"/>
+      <c r="C2" s="70"/>
+      <c r="D2" s="70"/>
+      <c r="E2" s="70"/>
+      <c r="F2" s="70"/>
+      <c r="G2" s="70"/>
+      <c r="H2" s="70"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
@@ -3000,16 +3357,16 @@
       </c>
     </row>
     <row r="10" spans="1:8" s="4" customFormat="1" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="77" t="s">
+      <c r="A10" s="79" t="s">
         <v>43</v>
       </c>
-      <c r="B10" s="77"/>
-      <c r="C10" s="77"/>
-      <c r="D10" s="77"/>
-      <c r="E10" s="77"/>
-      <c r="F10" s="77"/>
-      <c r="G10" s="77"/>
-      <c r="H10" s="77"/>
+      <c r="B10" s="79"/>
+      <c r="C10" s="79"/>
+      <c r="D10" s="79"/>
+      <c r="E10" s="79"/>
+      <c r="F10" s="79"/>
+      <c r="G10" s="79"/>
+      <c r="H10" s="79"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
@@ -3162,7 +3519,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44D7E2A8-7038-4E8B-9878-8235EBDD31DB}">
   <dimension ref="A1:K45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
@@ -3179,21 +3536,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="59" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="82" t="s">
+      <c r="A1" s="67" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="80" t="s">
         <v>96</v>
       </c>
-      <c r="C1" s="82"/>
-      <c r="D1" s="82"/>
+      <c r="C1" s="80"/>
+      <c r="D1" s="80"/>
       <c r="E1" s="18" t="s">
         <v>97</v>
       </c>
-      <c r="F1" s="82" t="s">
+      <c r="F1" s="80" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="82"/>
+      <c r="G1" s="80"/>
       <c r="H1" s="37" t="s">
         <v>117</v>
       </c>
@@ -3203,7 +3560,7 @@
       <c r="J1" s="28"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A2" s="59"/>
+      <c r="A2" s="67"/>
       <c r="B2" s="36" t="s">
         <v>93</v>
       </c>
@@ -3216,15 +3573,15 @@
       <c r="E2" s="18" t="s">
         <v>98</v>
       </c>
-      <c r="F2" s="82"/>
-      <c r="G2" s="82"/>
+      <c r="F2" s="80"/>
+      <c r="G2" s="80"/>
       <c r="H2" s="21" t="s">
         <v>135</v>
       </c>
-      <c r="I2" s="79" t="s">
+      <c r="I2" s="88" t="s">
         <v>137</v>
       </c>
-      <c r="J2" s="79"/>
+      <c r="J2" s="88"/>
       <c r="K2" s="21" t="s">
         <v>141</v>
       </c>
@@ -3245,17 +3602,17 @@
       <c r="E3" s="24" t="b">
         <v>1</v>
       </c>
-      <c r="F3" s="80" t="s">
+      <c r="F3" s="87" t="s">
         <v>106</v>
       </c>
-      <c r="G3" s="80"/>
+      <c r="G3" s="87"/>
       <c r="H3" s="21" t="s">
         <v>134</v>
       </c>
-      <c r="I3" s="79" t="s">
+      <c r="I3" s="88" t="s">
         <v>138</v>
       </c>
-      <c r="J3" s="79"/>
+      <c r="J3" s="88"/>
       <c r="K3" s="21" t="s">
         <v>142</v>
       </c>
@@ -3276,17 +3633,17 @@
       <c r="E4" s="24" t="b">
         <v>1</v>
       </c>
-      <c r="F4" s="87" t="s">
+      <c r="F4" s="86" t="s">
         <v>107</v>
       </c>
-      <c r="G4" s="87"/>
+      <c r="G4" s="86"/>
       <c r="H4" s="21" t="s">
         <v>133</v>
       </c>
-      <c r="I4" s="79" t="s">
+      <c r="I4" s="88" t="s">
         <v>139</v>
       </c>
-      <c r="J4" s="79"/>
+      <c r="J4" s="88"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="24">
@@ -3304,17 +3661,17 @@
       <c r="E5" s="24" t="b">
         <v>1</v>
       </c>
-      <c r="F5" s="86" t="s">
+      <c r="F5" s="85" t="s">
         <v>108</v>
       </c>
-      <c r="G5" s="86"/>
+      <c r="G5" s="85"/>
       <c r="H5" s="21" t="s">
         <v>132</v>
       </c>
-      <c r="I5" s="79" t="s">
+      <c r="I5" s="88" t="s">
         <v>140</v>
       </c>
-      <c r="J5" s="79"/>
+      <c r="J5" s="88"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="24">
@@ -3326,16 +3683,16 @@
       <c r="C6" s="24">
         <v>550</v>
       </c>
-      <c r="D6" s="97">
+      <c r="D6" s="58">
         <v>2500.0100000000002</v>
       </c>
       <c r="E6" s="24" t="b">
         <v>0</v>
       </c>
-      <c r="F6" s="85" t="s">
+      <c r="F6" s="84" t="s">
         <v>109</v>
       </c>
-      <c r="G6" s="85"/>
+      <c r="G6" s="84"/>
       <c r="I6" s="28"/>
       <c r="J6" s="28"/>
     </row>
@@ -3383,17 +3740,17 @@
       <c r="E8" s="24" t="b">
         <v>0</v>
       </c>
-      <c r="F8" s="84" t="s">
+      <c r="F8" s="83" t="s">
         <v>110</v>
       </c>
-      <c r="G8" s="84"/>
+      <c r="G8" s="83"/>
       <c r="H8" s="21" t="s">
         <v>130</v>
       </c>
-      <c r="I8" s="79" t="s">
+      <c r="I8" s="88" t="s">
         <v>145</v>
       </c>
-      <c r="J8" s="79"/>
+      <c r="J8" s="88"/>
       <c r="K8" s="21" t="s">
         <v>150</v>
       </c>
@@ -3414,17 +3771,17 @@
       <c r="E9" s="24" t="b">
         <v>0</v>
       </c>
-      <c r="F9" s="83" t="s">
+      <c r="F9" s="82" t="s">
         <v>111</v>
       </c>
-      <c r="G9" s="83"/>
+      <c r="G9" s="82"/>
       <c r="H9" s="21" t="s">
         <v>132</v>
       </c>
-      <c r="I9" s="79" t="s">
+      <c r="I9" s="88" t="s">
         <v>146</v>
       </c>
-      <c r="J9" s="79"/>
+      <c r="J9" s="88"/>
       <c r="K9" s="21" t="s">
         <v>151</v>
       </c>
@@ -3452,10 +3809,10 @@
       <c r="H10" s="21" t="s">
         <v>131</v>
       </c>
-      <c r="I10" s="79" t="s">
+      <c r="I10" s="88" t="s">
         <v>147</v>
       </c>
-      <c r="J10" s="79"/>
+      <c r="J10" s="88"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" s="24">
@@ -3473,17 +3830,17 @@
       <c r="E11" s="44" t="b">
         <v>0</v>
       </c>
-      <c r="F11" s="78" t="s">
+      <c r="F11" s="89" t="s">
         <v>24</v>
       </c>
-      <c r="G11" s="78"/>
+      <c r="G11" s="89"/>
       <c r="H11" s="21" t="s">
         <v>133</v>
       </c>
-      <c r="I11" s="79" t="s">
+      <c r="I11" s="88" t="s">
         <v>148</v>
       </c>
-      <c r="J11" s="79"/>
+      <c r="J11" s="88"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" s="24">
@@ -3501,17 +3858,17 @@
       <c r="E12" s="44" t="b">
         <v>0</v>
       </c>
-      <c r="F12" s="78" t="s">
+      <c r="F12" s="89" t="s">
         <v>24</v>
       </c>
-      <c r="G12" s="78"/>
+      <c r="G12" s="89"/>
       <c r="H12" s="21" t="s">
         <v>134</v>
       </c>
-      <c r="I12" s="79" t="s">
+      <c r="I12" s="88" t="s">
         <v>149</v>
       </c>
-      <c r="J12" s="79"/>
+      <c r="J12" s="88"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" s="24">
@@ -3529,10 +3886,10 @@
       <c r="E13" s="44" t="b">
         <v>0</v>
       </c>
-      <c r="F13" s="78" t="s">
+      <c r="F13" s="89" t="s">
         <v>24</v>
       </c>
-      <c r="G13" s="78"/>
+      <c r="G13" s="89"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" s="24">
@@ -3550,10 +3907,10 @@
       <c r="E14" s="44" t="b">
         <v>0</v>
       </c>
-      <c r="F14" s="78" t="s">
+      <c r="F14" s="89" t="s">
         <v>24</v>
       </c>
-      <c r="G14" s="78"/>
+      <c r="G14" s="89"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" s="24">
@@ -3567,10 +3924,10 @@
         <v>9000.01</v>
       </c>
       <c r="E15" s="24"/>
-      <c r="F15" s="78" t="s">
+      <c r="F15" s="89" t="s">
         <v>24</v>
       </c>
-      <c r="G15" s="78"/>
+      <c r="G15" s="89"/>
       <c r="J15" s="28"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.3">
@@ -3585,10 +3942,10 @@
         <v>6500.01</v>
       </c>
       <c r="E16" s="24"/>
-      <c r="F16" s="78" t="s">
+      <c r="F16" s="89" t="s">
         <v>24</v>
       </c>
-      <c r="G16" s="78"/>
+      <c r="G16" s="89"/>
       <c r="J16" s="28"/>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.3">
@@ -3603,10 +3960,10 @@
         <v>2499.9899999999998</v>
       </c>
       <c r="E17" s="24"/>
-      <c r="F17" s="78" t="s">
+      <c r="F17" s="89" t="s">
         <v>24</v>
       </c>
-      <c r="G17" s="78"/>
+      <c r="G17" s="89"/>
       <c r="J17" s="28"/>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.3">
@@ -3621,10 +3978,10 @@
         <v>6500.01</v>
       </c>
       <c r="E18" s="24"/>
-      <c r="F18" s="78" t="s">
+      <c r="F18" s="89" t="s">
         <v>24</v>
       </c>
-      <c r="G18" s="78"/>
+      <c r="G18" s="89"/>
       <c r="J18" s="28"/>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.3">
@@ -3639,10 +3996,10 @@
         <v>2499.9899999999998</v>
       </c>
       <c r="E19" s="24"/>
-      <c r="F19" s="78" t="s">
+      <c r="F19" s="89" t="s">
         <v>24</v>
       </c>
-      <c r="G19" s="78"/>
+      <c r="G19" s="89"/>
       <c r="J19" s="28"/>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.3">
@@ -3724,10 +4081,10 @@
       <c r="E30" s="21" t="s">
         <v>135</v>
       </c>
-      <c r="F30" s="79" t="s">
+      <c r="F30" s="88" t="s">
         <v>137</v>
       </c>
-      <c r="G30" s="79"/>
+      <c r="G30" s="88"/>
       <c r="H30" s="21" t="s">
         <v>141</v>
       </c>
@@ -3742,10 +4099,10 @@
       <c r="E31" s="21" t="s">
         <v>134</v>
       </c>
-      <c r="F31" s="79" t="s">
+      <c r="F31" s="88" t="s">
         <v>138</v>
       </c>
-      <c r="G31" s="79"/>
+      <c r="G31" s="88"/>
       <c r="H31" s="21" t="s">
         <v>142</v>
       </c>
@@ -3760,10 +4117,10 @@
       <c r="E32" s="21" t="s">
         <v>133</v>
       </c>
-      <c r="F32" s="79" t="s">
+      <c r="F32" s="88" t="s">
         <v>139</v>
       </c>
-      <c r="G32" s="79"/>
+      <c r="G32" s="88"/>
     </row>
     <row r="33" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B33" s="21" t="s">
@@ -3775,10 +4132,10 @@
       <c r="E33" s="21" t="s">
         <v>132</v>
       </c>
-      <c r="F33" s="79" t="s">
+      <c r="F33" s="88" t="s">
         <v>140</v>
       </c>
-      <c r="G33" s="79"/>
+      <c r="G33" s="88"/>
     </row>
     <row r="34" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B34" s="21" t="s">
@@ -3808,10 +4165,10 @@
       <c r="E38" s="21" t="s">
         <v>130</v>
       </c>
-      <c r="F38" s="79" t="s">
+      <c r="F38" s="88" t="s">
         <v>145</v>
       </c>
-      <c r="G38" s="79"/>
+      <c r="G38" s="88"/>
       <c r="H38" s="21" t="s">
         <v>150</v>
       </c>
@@ -3820,10 +4177,10 @@
       <c r="E39" s="21" t="s">
         <v>132</v>
       </c>
-      <c r="F39" s="79" t="s">
+      <c r="F39" s="88" t="s">
         <v>146</v>
       </c>
-      <c r="G39" s="79"/>
+      <c r="G39" s="88"/>
       <c r="H39" s="21" t="s">
         <v>151</v>
       </c>
@@ -3832,28 +4189,28 @@
       <c r="E40" s="21" t="s">
         <v>131</v>
       </c>
-      <c r="F40" s="79" t="s">
+      <c r="F40" s="88" t="s">
         <v>147</v>
       </c>
-      <c r="G40" s="79"/>
+      <c r="G40" s="88"/>
     </row>
     <row r="41" spans="2:8" x14ac:dyDescent="0.3">
       <c r="E41" s="21" t="s">
         <v>133</v>
       </c>
-      <c r="F41" s="79" t="s">
+      <c r="F41" s="88" t="s">
         <v>148</v>
       </c>
-      <c r="G41" s="79"/>
+      <c r="G41" s="88"/>
     </row>
     <row r="42" spans="2:8" x14ac:dyDescent="0.3">
       <c r="E42" s="21" t="s">
         <v>134</v>
       </c>
-      <c r="F42" s="79" t="s">
+      <c r="F42" s="88" t="s">
         <v>149</v>
       </c>
-      <c r="G42" s="79"/>
+      <c r="G42" s="88"/>
     </row>
     <row r="43" spans="2:8" x14ac:dyDescent="0.3">
       <c r="F43" s="21"/>
@@ -3866,6 +4223,33 @@
     </row>
   </sheetData>
   <mergeCells count="38">
+    <mergeCell ref="I9:J9"/>
+    <mergeCell ref="I10:J10"/>
+    <mergeCell ref="I11:J11"/>
+    <mergeCell ref="I12:J12"/>
+    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="F12:G12"/>
+    <mergeCell ref="F42:G42"/>
+    <mergeCell ref="F41:G41"/>
+    <mergeCell ref="F40:G40"/>
+    <mergeCell ref="F39:G39"/>
+    <mergeCell ref="F38:G38"/>
+    <mergeCell ref="I2:J2"/>
+    <mergeCell ref="I3:J3"/>
+    <mergeCell ref="I4:J4"/>
+    <mergeCell ref="I5:J5"/>
+    <mergeCell ref="I8:J8"/>
+    <mergeCell ref="F33:G33"/>
+    <mergeCell ref="F32:G32"/>
+    <mergeCell ref="F31:G31"/>
+    <mergeCell ref="F30:G30"/>
+    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="F15:G15"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="F17:G17"/>
+    <mergeCell ref="F18:G18"/>
+    <mergeCell ref="F19:G19"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:D1"/>
     <mergeCell ref="F1:G2"/>
@@ -3877,33 +4261,6 @@
     <mergeCell ref="F4:G4"/>
     <mergeCell ref="F3:G3"/>
     <mergeCell ref="F7:G7"/>
-    <mergeCell ref="F33:G33"/>
-    <mergeCell ref="F32:G32"/>
-    <mergeCell ref="F31:G31"/>
-    <mergeCell ref="F30:G30"/>
-    <mergeCell ref="F13:G13"/>
-    <mergeCell ref="F14:G14"/>
-    <mergeCell ref="F15:G15"/>
-    <mergeCell ref="F16:G16"/>
-    <mergeCell ref="I2:J2"/>
-    <mergeCell ref="I3:J3"/>
-    <mergeCell ref="I4:J4"/>
-    <mergeCell ref="I5:J5"/>
-    <mergeCell ref="I8:J8"/>
-    <mergeCell ref="F42:G42"/>
-    <mergeCell ref="F41:G41"/>
-    <mergeCell ref="F40:G40"/>
-    <mergeCell ref="F39:G39"/>
-    <mergeCell ref="F38:G38"/>
-    <mergeCell ref="F17:G17"/>
-    <mergeCell ref="F18:G18"/>
-    <mergeCell ref="F19:G19"/>
-    <mergeCell ref="I9:J9"/>
-    <mergeCell ref="I10:J10"/>
-    <mergeCell ref="I11:J11"/>
-    <mergeCell ref="I12:J12"/>
-    <mergeCell ref="F11:G11"/>
-    <mergeCell ref="F12:G12"/>
   </mergeCells>
   <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3916,7 +4273,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCF6D9F7-D4E3-49EA-A4E4-B61C1736EDE1}">
   <dimension ref="A1:J30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A3" workbookViewId="0">
       <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
@@ -3931,58 +4288,58 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="59" t="s">
+      <c r="A1" s="67" t="s">
         <v>169</v>
       </c>
-      <c r="B1" s="60" t="s">
+      <c r="B1" s="68" t="s">
         <v>96</v>
       </c>
-      <c r="C1" s="60"/>
-      <c r="D1" s="60"/>
+      <c r="C1" s="68"/>
+      <c r="D1" s="68"/>
       <c r="E1" s="20" t="s">
         <v>97</v>
       </c>
-      <c r="F1" s="59" t="s">
+      <c r="F1" s="67" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="59"/>
-      <c r="H1" s="82" t="s">
+      <c r="G1" s="67"/>
+      <c r="H1" s="80" t="s">
         <v>155</v>
       </c>
-      <c r="I1" s="82"/>
-      <c r="J1" s="82"/>
+      <c r="I1" s="80"/>
+      <c r="J1" s="80"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A2" s="59"/>
-      <c r="B2" s="59" t="s">
+      <c r="A2" s="67"/>
+      <c r="B2" s="67" t="s">
         <v>152</v>
       </c>
-      <c r="C2" s="95" t="s">
+      <c r="C2" s="92" t="s">
         <v>153</v>
       </c>
-      <c r="D2" s="59" t="s">
+      <c r="D2" s="67" t="s">
         <v>154</v>
       </c>
-      <c r="E2" s="82" t="s">
+      <c r="E2" s="80" t="s">
         <v>170</v>
       </c>
-      <c r="F2" s="59"/>
-      <c r="G2" s="59"/>
-      <c r="H2" s="82"/>
-      <c r="I2" s="82"/>
-      <c r="J2" s="82"/>
+      <c r="F2" s="67"/>
+      <c r="G2" s="67"/>
+      <c r="H2" s="80"/>
+      <c r="I2" s="80"/>
+      <c r="J2" s="80"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A3" s="59"/>
-      <c r="B3" s="59"/>
-      <c r="C3" s="95"/>
-      <c r="D3" s="59"/>
-      <c r="E3" s="82"/>
-      <c r="F3" s="59"/>
-      <c r="G3" s="59"/>
-      <c r="H3" s="82"/>
-      <c r="I3" s="82"/>
-      <c r="J3" s="82"/>
+      <c r="A3" s="67"/>
+      <c r="B3" s="67"/>
+      <c r="C3" s="92"/>
+      <c r="D3" s="67"/>
+      <c r="E3" s="80"/>
+      <c r="F3" s="67"/>
+      <c r="G3" s="67"/>
+      <c r="H3" s="80"/>
+      <c r="I3" s="80"/>
+      <c r="J3" s="80"/>
     </row>
     <row r="4" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="24">
@@ -4000,13 +4357,13 @@
       <c r="E4" s="49" t="s">
         <v>164</v>
       </c>
-      <c r="F4" s="92" t="s">
+      <c r="F4" s="93" t="s">
         <v>156</v>
       </c>
-      <c r="G4" s="92"/>
-      <c r="H4" s="90"/>
-      <c r="I4" s="90"/>
-      <c r="J4" s="90"/>
+      <c r="G4" s="93"/>
+      <c r="H4" s="91"/>
+      <c r="I4" s="91"/>
+      <c r="J4" s="91"/>
     </row>
     <row r="5" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A5" s="24">
@@ -4024,13 +4381,13 @@
       <c r="E5" s="49" t="s">
         <v>165</v>
       </c>
-      <c r="F5" s="93" t="s">
+      <c r="F5" s="94" t="s">
         <v>157</v>
       </c>
-      <c r="G5" s="93"/>
-      <c r="H5" s="90"/>
-      <c r="I5" s="90"/>
-      <c r="J5" s="90"/>
+      <c r="G5" s="94"/>
+      <c r="H5" s="91"/>
+      <c r="I5" s="91"/>
+      <c r="J5" s="91"/>
     </row>
     <row r="6" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A6" s="24">
@@ -4048,13 +4405,13 @@
       <c r="E6" s="49" t="s">
         <v>166</v>
       </c>
-      <c r="F6" s="94" t="s">
+      <c r="F6" s="95" t="s">
         <v>158</v>
       </c>
-      <c r="G6" s="94"/>
-      <c r="H6" s="90"/>
-      <c r="I6" s="90"/>
-      <c r="J6" s="90"/>
+      <c r="G6" s="95"/>
+      <c r="H6" s="91"/>
+      <c r="I6" s="91"/>
+      <c r="J6" s="91"/>
     </row>
     <row r="7" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A7" s="24">
@@ -4072,13 +4429,13 @@
       <c r="E7" s="49" t="s">
         <v>167</v>
       </c>
-      <c r="F7" s="91" t="s">
+      <c r="F7" s="90" t="s">
         <v>159</v>
       </c>
-      <c r="G7" s="91"/>
-      <c r="H7" s="90"/>
-      <c r="I7" s="90"/>
-      <c r="J7" s="90"/>
+      <c r="G7" s="90"/>
+      <c r="H7" s="91"/>
+      <c r="I7" s="91"/>
+      <c r="J7" s="91"/>
     </row>
     <row r="8" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A8" s="24">
@@ -4096,13 +4453,13 @@
       <c r="E8" s="49" t="s">
         <v>167</v>
       </c>
-      <c r="F8" s="91" t="s">
+      <c r="F8" s="90" t="s">
         <v>160</v>
       </c>
-      <c r="G8" s="91"/>
-      <c r="H8" s="90"/>
-      <c r="I8" s="90"/>
-      <c r="J8" s="90"/>
+      <c r="G8" s="90"/>
+      <c r="H8" s="91"/>
+      <c r="I8" s="91"/>
+      <c r="J8" s="91"/>
     </row>
     <row r="9" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A9" s="24">
@@ -4120,13 +4477,13 @@
       <c r="E9" s="49" t="s">
         <v>167</v>
       </c>
-      <c r="F9" s="91" t="s">
+      <c r="F9" s="90" t="s">
         <v>161</v>
       </c>
-      <c r="G9" s="91"/>
-      <c r="H9" s="90"/>
-      <c r="I9" s="90"/>
-      <c r="J9" s="90"/>
+      <c r="G9" s="90"/>
+      <c r="H9" s="91"/>
+      <c r="I9" s="91"/>
+      <c r="J9" s="91"/>
     </row>
     <row r="10" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A10" s="24">
@@ -4144,13 +4501,13 @@
       <c r="E10" s="49" t="s">
         <v>167</v>
       </c>
-      <c r="F10" s="91" t="s">
+      <c r="F10" s="90" t="s">
         <v>162</v>
       </c>
-      <c r="G10" s="91"/>
-      <c r="H10" s="90"/>
-      <c r="I10" s="90"/>
-      <c r="J10" s="90"/>
+      <c r="G10" s="90"/>
+      <c r="H10" s="91"/>
+      <c r="I10" s="91"/>
+      <c r="J10" s="91"/>
     </row>
     <row r="11" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A11" s="24">
@@ -4168,13 +4525,13 @@
       <c r="E11" s="49" t="s">
         <v>167</v>
       </c>
-      <c r="F11" s="91" t="s">
+      <c r="F11" s="90" t="s">
         <v>163</v>
       </c>
-      <c r="G11" s="91"/>
-      <c r="H11" s="90"/>
-      <c r="I11" s="90"/>
-      <c r="J11" s="90"/>
+      <c r="G11" s="90"/>
+      <c r="H11" s="91"/>
+      <c r="I11" s="91"/>
+      <c r="J11" s="91"/>
     </row>
     <row r="12" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A12" s="24">
@@ -4189,16 +4546,16 @@
       <c r="D12" s="52">
         <v>3500</v>
       </c>
-      <c r="E12" s="96" t="s">
+      <c r="E12" s="57" t="s">
         <v>167</v>
       </c>
-      <c r="F12" s="91" t="s">
+      <c r="F12" s="90" t="s">
         <v>24</v>
       </c>
-      <c r="G12" s="91"/>
-      <c r="H12" s="90"/>
-      <c r="I12" s="90"/>
-      <c r="J12" s="90"/>
+      <c r="G12" s="90"/>
+      <c r="H12" s="91"/>
+      <c r="I12" s="91"/>
+      <c r="J12" s="91"/>
     </row>
     <row r="13" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A13" s="24">
@@ -4213,16 +4570,16 @@
       <c r="D13" s="52">
         <v>3500</v>
       </c>
-      <c r="E13" s="96" t="s">
+      <c r="E13" s="57" t="s">
         <v>167</v>
       </c>
-      <c r="F13" s="91" t="s">
+      <c r="F13" s="90" t="s">
         <v>24</v>
       </c>
-      <c r="G13" s="91"/>
-      <c r="H13" s="90"/>
-      <c r="I13" s="90"/>
-      <c r="J13" s="90"/>
+      <c r="G13" s="90"/>
+      <c r="H13" s="91"/>
+      <c r="I13" s="91"/>
+      <c r="J13" s="91"/>
     </row>
     <row r="14" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A14" s="24">
@@ -4237,16 +4594,16 @@
       <c r="D14" s="54" t="s">
         <v>168</v>
       </c>
-      <c r="E14" s="96" t="s">
+      <c r="E14" s="57" t="s">
         <v>167</v>
       </c>
-      <c r="F14" s="91" t="s">
+      <c r="F14" s="90" t="s">
         <v>24</v>
       </c>
-      <c r="G14" s="91"/>
-      <c r="H14" s="90"/>
-      <c r="I14" s="90"/>
-      <c r="J14" s="90"/>
+      <c r="G14" s="90"/>
+      <c r="H14" s="91"/>
+      <c r="I14" s="91"/>
+      <c r="J14" s="91"/>
     </row>
     <row r="15" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A15" s="24">
@@ -4261,16 +4618,16 @@
       <c r="D15" s="55">
         <v>10000</v>
       </c>
-      <c r="E15" s="96" t="s">
+      <c r="E15" s="57" t="s">
         <v>167</v>
       </c>
-      <c r="F15" s="91" t="s">
+      <c r="F15" s="90" t="s">
         <v>24</v>
       </c>
-      <c r="G15" s="91"/>
-      <c r="H15" s="90"/>
-      <c r="I15" s="90"/>
-      <c r="J15" s="90"/>
+      <c r="G15" s="90"/>
+      <c r="H15" s="91"/>
+      <c r="I15" s="91"/>
+      <c r="J15" s="91"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C16" s="42"/>
@@ -4294,10 +4651,10 @@
       <c r="A19" t="s">
         <v>172</v>
       </c>
-      <c r="B19" s="88" t="s">
+      <c r="B19" s="96" t="s">
         <v>178</v>
       </c>
-      <c r="C19" s="88"/>
+      <c r="C19" s="96"/>
       <c r="D19" s="43" t="s">
         <v>194</v>
       </c>
@@ -4306,10 +4663,10 @@
       <c r="A20" t="s">
         <v>173</v>
       </c>
-      <c r="B20" s="88" t="s">
+      <c r="B20" s="96" t="s">
         <v>177</v>
       </c>
-      <c r="C20" s="88"/>
+      <c r="C20" s="96"/>
       <c r="D20" s="43" t="s">
         <v>195</v>
       </c>
@@ -4318,30 +4675,30 @@
       <c r="A21" t="s">
         <v>174</v>
       </c>
-      <c r="B21" s="88" t="s">
+      <c r="B21" s="96" t="s">
         <v>179</v>
       </c>
-      <c r="C21" s="88"/>
+      <c r="C21" s="96"/>
       <c r="D21" s="43"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" s="56" t="s">
         <v>175</v>
       </c>
-      <c r="B22" s="89" t="s">
+      <c r="B22" s="97" t="s">
         <v>180</v>
       </c>
-      <c r="C22" s="89"/>
+      <c r="C22" s="97"/>
       <c r="D22" s="43"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" s="56" t="s">
         <v>176</v>
       </c>
-      <c r="B23" s="89" t="s">
+      <c r="B23" s="97" t="s">
         <v>181</v>
       </c>
-      <c r="C23" s="89"/>
+      <c r="C23" s="97"/>
       <c r="D23" s="43"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
@@ -4356,10 +4713,10 @@
       <c r="A26" t="s">
         <v>172</v>
       </c>
-      <c r="B26" s="88" t="s">
+      <c r="B26" s="96" t="s">
         <v>184</v>
       </c>
-      <c r="C26" s="88"/>
+      <c r="C26" s="96"/>
       <c r="D26" s="1" t="s">
         <v>190</v>
       </c>
@@ -4368,10 +4725,10 @@
       <c r="A27" t="s">
         <v>173</v>
       </c>
-      <c r="B27" s="88" t="s">
+      <c r="B27" s="96" t="s">
         <v>186</v>
       </c>
-      <c r="C27" s="88"/>
+      <c r="C27" s="96"/>
       <c r="D27" s="1" t="s">
         <v>192</v>
       </c>
@@ -4380,10 +4737,10 @@
       <c r="A28" t="s">
         <v>174</v>
       </c>
-      <c r="B28" s="88" t="s">
+      <c r="B28" s="96" t="s">
         <v>185</v>
       </c>
-      <c r="C28" s="88"/>
+      <c r="C28" s="96"/>
       <c r="D28" s="1" t="s">
         <v>191</v>
       </c>
@@ -4392,10 +4749,10 @@
       <c r="A29" t="s">
         <v>175</v>
       </c>
-      <c r="B29" s="88" t="s">
+      <c r="B29" s="96" t="s">
         <v>187</v>
       </c>
-      <c r="C29" s="88"/>
+      <c r="C29" s="96"/>
       <c r="D29" s="1" t="s">
         <v>189</v>
       </c>
@@ -4404,16 +4761,42 @@
       <c r="A30" t="s">
         <v>176</v>
       </c>
-      <c r="B30" s="88" t="s">
+      <c r="B30" s="96" t="s">
         <v>188</v>
       </c>
-      <c r="C30" s="88"/>
+      <c r="C30" s="96"/>
       <c r="D30" s="1" t="s">
         <v>193</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="42">
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="F9:G9"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="H12:J12"/>
+    <mergeCell ref="H13:J13"/>
+    <mergeCell ref="H14:J14"/>
+    <mergeCell ref="H15:J15"/>
+    <mergeCell ref="F12:G12"/>
+    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="F15:G15"/>
+    <mergeCell ref="H4:J4"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="F7:G7"/>
     <mergeCell ref="F8:G8"/>
     <mergeCell ref="F1:G3"/>
     <mergeCell ref="H1:J3"/>
@@ -4430,36 +4813,291 @@
     <mergeCell ref="D2:D3"/>
     <mergeCell ref="E2:E3"/>
     <mergeCell ref="B1:D1"/>
-    <mergeCell ref="H4:J4"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="F5:G5"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="F7:G7"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="F9:G9"/>
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="F11:G11"/>
-    <mergeCell ref="H12:J12"/>
-    <mergeCell ref="H13:J13"/>
-    <mergeCell ref="H14:J14"/>
-    <mergeCell ref="H15:J15"/>
-    <mergeCell ref="F12:G12"/>
-    <mergeCell ref="F13:G13"/>
-    <mergeCell ref="F14:G14"/>
-    <mergeCell ref="F15:G15"/>
-    <mergeCell ref="B28:C28"/>
-    <mergeCell ref="B29:C29"/>
-    <mergeCell ref="B30:C30"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="B27:C27"/>
   </mergeCells>
   <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83FABE2F-9C9C-4A9F-9234-D36F5EBE9127}">
+  <dimension ref="A1:N13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L7" sqref="L7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="8.88671875" style="100"/>
+    <col min="2" max="3" width="8.88671875" style="102"/>
+    <col min="4" max="4" width="10.109375" style="99" customWidth="1"/>
+    <col min="5" max="5" width="11.44140625" style="99" customWidth="1"/>
+    <col min="8" max="8" width="11.33203125" customWidth="1"/>
+    <col min="9" max="9" width="11.5546875" customWidth="1"/>
+    <col min="10" max="10" width="9.21875" customWidth="1"/>
+    <col min="11" max="11" width="9.77734375" customWidth="1"/>
+    <col min="12" max="13" width="9.5546875" customWidth="1"/>
+    <col min="14" max="14" width="10.5546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="74" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="101" t="s">
+        <v>96</v>
+      </c>
+      <c r="C1" s="101" t="s">
+        <v>196</v>
+      </c>
+      <c r="D1" s="74" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="74"/>
+    </row>
+    <row r="2" spans="1:14" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="74"/>
+      <c r="B2" s="101" t="s">
+        <v>197</v>
+      </c>
+      <c r="C2" s="101" t="s">
+        <v>198</v>
+      </c>
+      <c r="D2" s="74"/>
+      <c r="E2" s="74"/>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A3" s="103">
+        <v>1</v>
+      </c>
+      <c r="B3" s="104" t="s">
+        <v>206</v>
+      </c>
+      <c r="C3" s="105">
+        <v>6</v>
+      </c>
+      <c r="D3" s="106" t="s">
+        <v>207</v>
+      </c>
+      <c r="E3" s="107"/>
+      <c r="G3" t="s">
+        <v>7</v>
+      </c>
+      <c r="H3" s="98" t="s">
+        <v>199</v>
+      </c>
+      <c r="I3" s="98" t="s">
+        <v>200</v>
+      </c>
+      <c r="J3" t="s">
+        <v>201</v>
+      </c>
+      <c r="K3" t="s">
+        <v>202</v>
+      </c>
+      <c r="L3" t="s">
+        <v>203</v>
+      </c>
+      <c r="M3" t="s">
+        <v>204</v>
+      </c>
+      <c r="N3" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A4" s="103">
+        <v>2</v>
+      </c>
+      <c r="B4" s="104" t="s">
+        <v>214</v>
+      </c>
+      <c r="C4" s="105">
+        <v>7</v>
+      </c>
+      <c r="D4" s="108" t="s">
+        <v>208</v>
+      </c>
+      <c r="E4" s="109"/>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A5" s="103">
+        <v>3</v>
+      </c>
+      <c r="B5" s="105">
+        <v>2</v>
+      </c>
+      <c r="C5" s="105">
+        <v>0</v>
+      </c>
+      <c r="D5" s="110" t="s">
+        <v>209</v>
+      </c>
+      <c r="E5" s="111"/>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A6" s="103">
+        <v>4</v>
+      </c>
+      <c r="B6" s="105">
+        <v>6</v>
+      </c>
+      <c r="C6" s="105">
+        <v>0</v>
+      </c>
+      <c r="D6" s="112" t="s">
+        <v>210</v>
+      </c>
+      <c r="E6" s="112"/>
+      <c r="K6" s="35" t="s">
+        <v>215</v>
+      </c>
+      <c r="L6" s="35" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A7" s="103">
+        <v>5</v>
+      </c>
+      <c r="B7" s="105">
+        <v>8</v>
+      </c>
+      <c r="C7" s="105">
+        <v>6</v>
+      </c>
+      <c r="D7" s="113" t="s">
+        <v>211</v>
+      </c>
+      <c r="E7" s="113"/>
+      <c r="K7" t="s">
+        <v>216</v>
+      </c>
+      <c r="L7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A8" s="103">
+        <v>6</v>
+      </c>
+      <c r="B8" s="105">
+        <v>9</v>
+      </c>
+      <c r="C8" s="105">
+        <v>6</v>
+      </c>
+      <c r="D8" s="114" t="s">
+        <v>212</v>
+      </c>
+      <c r="E8" s="114"/>
+      <c r="K8" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A9" s="103">
+        <v>7</v>
+      </c>
+      <c r="B9" s="105">
+        <v>9.01</v>
+      </c>
+      <c r="C9" s="105">
+        <v>7</v>
+      </c>
+      <c r="D9" s="107" t="s">
+        <v>213</v>
+      </c>
+      <c r="E9" s="107"/>
+      <c r="K9" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A10" s="103">
+        <v>8</v>
+      </c>
+      <c r="B10" s="105">
+        <v>-2</v>
+      </c>
+      <c r="C10" s="115">
+        <v>6</v>
+      </c>
+      <c r="D10" s="116" t="s">
+        <v>24</v>
+      </c>
+      <c r="E10" s="116"/>
+      <c r="K10" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A11" s="103">
+        <v>9</v>
+      </c>
+      <c r="B11" s="105">
+        <v>10</v>
+      </c>
+      <c r="C11" s="115">
+        <v>7</v>
+      </c>
+      <c r="D11" s="116" t="s">
+        <v>24</v>
+      </c>
+      <c r="E11" s="116"/>
+      <c r="K11" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A12" s="103">
+        <v>10</v>
+      </c>
+      <c r="B12" s="105"/>
+      <c r="C12" s="105"/>
+      <c r="D12" s="116" t="s">
+        <v>24</v>
+      </c>
+      <c r="E12" s="116"/>
+      <c r="K12" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A13" s="103">
+        <v>11</v>
+      </c>
+      <c r="B13" s="105"/>
+      <c r="C13" s="105"/>
+      <c r="D13" s="116" t="s">
+        <v>24</v>
+      </c>
+      <c r="E13" s="116"/>
+      <c r="K13" t="s">
+        <v>222</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="13">
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="D1:E2"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="D4:E4"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
ST homework 3 update Q5
</commit_message>
<xml_diff>
--- a/2020 Summer/CSE 5321 Software Testing/Homework 3/Homework-03.xlsx
+++ b/2020 Summer/CSE 5321 Software Testing/Homework 3/Homework-03.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gaura\Documents\Academic\UTA\2020 Summer\CSE 5321 Software Testing\Homework 3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{310D1D8D-8D13-4AC1-A348-E4544A415127}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAC4E226-CC76-46F5-AA25-F1FF0B1A12C7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="6" xr2:uid="{CA2C47C1-9B3A-4639-99C1-0BD544F6496B}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="376" uniqueCount="224">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="374" uniqueCount="246">
   <si>
     <t>Test Case Number</t>
   </si>
@@ -467,12 +467,6 @@
     <t>551, 6500.01</t>
   </si>
   <si>
-    <t>551, 6499.99</t>
-  </si>
-  <si>
-    <t>551, 9000.01</t>
-  </si>
-  <si>
     <t>550, 6500.01</t>
   </si>
   <si>
@@ -494,15 +488,9 @@
     <t>1000, 2500.01</t>
   </si>
   <si>
-    <t xml:space="preserve">1000, 2499.99 </t>
-  </si>
-  <si>
     <t>1001, 6500.01</t>
   </si>
   <si>
-    <t>1001, 2499.99</t>
-  </si>
-  <si>
     <t>TC 5</t>
   </si>
   <si>
@@ -698,14 +686,86 @@
     <t>-0.01</t>
   </si>
   <si>
-    <t>abcdef</t>
-  </si>
-  <si>
-    <t>TTTTTT</t>
+    <t>1001, 2500.00</t>
+  </si>
+  <si>
+    <t>551, 6500.00</t>
+  </si>
+  <si>
+    <t>551, 9000.00</t>
+  </si>
+  <si>
+    <t>1000, 2500.00</t>
+  </si>
+  <si>
+    <t>TC 7</t>
+  </si>
+  <si>
+    <t>TC 6</t>
+  </si>
+  <si>
+    <t>TC 1</t>
+  </si>
+  <si>
+    <t>TC 4</t>
+  </si>
+  <si>
+    <t>9-14 TTF</t>
+  </si>
+  <si>
+    <t>9-14 FTT</t>
+  </si>
+  <si>
+    <t>16-19 FTT</t>
+  </si>
+  <si>
+    <t>16-19 TFT</t>
+  </si>
+  <si>
+    <t>9-14 TFT</t>
+  </si>
+  <si>
+    <t>16-19 TTF</t>
+  </si>
+  <si>
+    <t>9-14 FTF</t>
+  </si>
+  <si>
+    <t>9-14 FFT</t>
+  </si>
+  <si>
+    <t>16-19 TTT</t>
+  </si>
+  <si>
+    <t>Extreme range memberPoints</t>
+  </si>
+  <si>
+    <t>Extreme range total</t>
+  </si>
+  <si>
+    <t>a+b</t>
+  </si>
+  <si>
+    <t>XF</t>
+  </si>
+  <si>
+    <t>UC</t>
+  </si>
+  <si>
+    <t>FX</t>
+  </si>
+  <si>
+    <t>Extreme range temp.</t>
+  </si>
+  <si>
+    <t>a+b+c+d+e+f</t>
+  </si>
+  <si>
+    <t>FFFFFF</t>
   </si>
   <si>
     <r>
-      <t>T</t>
+      <t>FFFFF</t>
     </r>
     <r>
       <rPr>
@@ -716,45 +776,12 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>F</t>
+      <t>T</t>
     </r>
+  </si>
+  <si>
     <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>TTTT</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>F</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>TTTTT</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>TT</t>
+      <t>FFFF</t>
     </r>
     <r>
       <rPr>
@@ -765,7 +792,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>F</t>
+      <t>T</t>
     </r>
     <r>
       <rPr>
@@ -775,12 +802,12 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>TTT</t>
+      <t>F</t>
     </r>
   </si>
   <si>
     <r>
-      <t>TTT</t>
+      <t>FFF</t>
     </r>
     <r>
       <rPr>
@@ -791,7 +818,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>F</t>
+      <t>T</t>
     </r>
     <r>
       <rPr>
@@ -801,12 +828,12 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>TT</t>
+      <t>FF</t>
     </r>
   </si>
   <si>
     <r>
-      <t>TTTT</t>
+      <t>FF</t>
     </r>
     <r>
       <rPr>
@@ -817,7 +844,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>F</t>
+      <t>T</t>
     </r>
     <r>
       <rPr>
@@ -827,12 +854,12 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>T</t>
+      <t>FFF</t>
     </r>
   </si>
   <si>
     <r>
-      <t>TTTTT</t>
+      <t>F</t>
     </r>
     <r>
       <rPr>
@@ -843,11 +870,50 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>F</t>
+      <t>T</t>
     </r>
-  </si>
-  <si>
-    <t>if (x &lt; -1.00 &amp;&amp; x &lt; 0.0 &amp;&amp; x &lt;= 2.0 &amp;&amp; x &lt;= 6.0 &amp;&amp; x &lt;= 8.0 &amp;&amp; x &lt;= 9.0)</t>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>FFFF</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>T</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>FFFFF</t>
+    </r>
+  </si>
+  <si>
+    <t>if (x &lt; -1.00 || x &lt; 0.0 || x &lt;= 2.0 || x &lt;= 6.0 || x &lt;= 8.0 || x &lt;= 9.0)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  </t>
+  </si>
+  <si>
+    <t>extreme value x</t>
   </si>
 </sst>
 </file>
@@ -860,7 +926,7 @@
     <numFmt numFmtId="165" formatCode="0.0"/>
     <numFmt numFmtId="166" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -920,35 +986,7 @@
     </font>
     <font>
       <sz val="12"/>
-      <color theme="8" tint="-0.249977111117893"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF33E7FF"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF7030A0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
       <color theme="9" tint="-0.249977111117893"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="7" tint="0.39997558519241921"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1008,8 +1046,56 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="9" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="8" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="7" tint="0.39997558519241921"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF33E7FF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF7030A0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1037,12 +1123,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1171,7 +1251,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="117">
+  <cellXfs count="127">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1285,7 +1365,7 @@
     <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1305,10 +1385,36 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="166" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1353,9 +1459,6 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1364,100 +1467,92 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="17" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="5" fillId="5" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1471,11 +1566,24 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1603,16 +1711,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>350521</xdr:colOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>358141</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>289560</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>6096</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>575998</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>22860</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1634,8 +1742,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9966961" y="0"/>
-          <a:ext cx="2377439" cy="4151376"/>
+          <a:off x="6888481" y="0"/>
+          <a:ext cx="2046657" cy="3573780"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1660,7 +1768,7 @@
       <xdr:col>15</xdr:col>
       <xdr:colOff>38100</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>128016</xdr:rowOff>
+      <xdr:rowOff>69401</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1700,15 +1808,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>106681</xdr:colOff>
+      <xdr:colOff>7621</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>167640</xdr:rowOff>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>617220</xdr:colOff>
+      <xdr:colOff>518160</xdr:colOff>
       <xdr:row>26</xdr:row>
-      <xdr:rowOff>112776</xdr:rowOff>
+      <xdr:rowOff>21336</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1730,7 +1838,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3764281" y="731520"/>
+          <a:off x="3924301" y="640080"/>
           <a:ext cx="2689859" cy="4151376"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -2067,23 +2175,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A1" s="67" t="s">
+      <c r="A1" s="77" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="68" t="s">
+      <c r="C1" s="78" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="68"/>
-      <c r="E1" s="61" t="s">
+      <c r="D1" s="78"/>
+      <c r="E1" s="71" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="62"/>
+      <c r="F1" s="72"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" s="67"/>
+      <c r="A2" s="77"/>
       <c r="B2" s="19" t="s">
         <v>2</v>
       </c>
@@ -2093,8 +2201,8 @@
       <c r="D2" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="63"/>
-      <c r="F2" s="64"/>
+      <c r="E2" s="73"/>
+      <c r="F2" s="74"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="22">
@@ -2109,10 +2217,10 @@
       <c r="D3" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="65" t="s">
+      <c r="E3" s="75" t="s">
         <v>16</v>
       </c>
-      <c r="F3" s="66"/>
+      <c r="F3" s="76"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="22">
@@ -2127,10 +2235,10 @@
       <c r="D4" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="E4" s="65" t="s">
+      <c r="E4" s="75" t="s">
         <v>17</v>
       </c>
-      <c r="F4" s="66"/>
+      <c r="F4" s="76"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="22">
@@ -2145,10 +2253,10 @@
       <c r="D5" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="E5" s="65" t="s">
+      <c r="E5" s="75" t="s">
         <v>18</v>
       </c>
-      <c r="F5" s="66"/>
+      <c r="F5" s="76"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="22">
@@ -2163,10 +2271,10 @@
       <c r="D6" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="E6" s="65" t="s">
+      <c r="E6" s="75" t="s">
         <v>19</v>
       </c>
-      <c r="F6" s="66"/>
+      <c r="F6" s="76"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="22">
@@ -2181,10 +2289,10 @@
       <c r="D7" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="E7" s="65" t="s">
+      <c r="E7" s="75" t="s">
         <v>20</v>
       </c>
-      <c r="F7" s="66"/>
+      <c r="F7" s="76"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="22">
@@ -2199,10 +2307,10 @@
       <c r="D8" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="E8" s="65" t="s">
+      <c r="E8" s="75" t="s">
         <v>21</v>
       </c>
-      <c r="F8" s="66"/>
+      <c r="F8" s="76"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="22">
@@ -2217,10 +2325,10 @@
       <c r="D9" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="E9" s="65" t="s">
+      <c r="E9" s="75" t="s">
         <v>22</v>
       </c>
-      <c r="F9" s="66"/>
+      <c r="F9" s="76"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="22">
@@ -2235,10 +2343,10 @@
       <c r="D10" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="E10" s="65" t="s">
+      <c r="E10" s="75" t="s">
         <v>23</v>
       </c>
-      <c r="F10" s="66"/>
+      <c r="F10" s="76"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="23">
@@ -2253,10 +2361,10 @@
       <c r="D11" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="E11" s="59" t="s">
+      <c r="E11" s="69" t="s">
         <v>24</v>
       </c>
-      <c r="F11" s="60"/>
+      <c r="F11" s="70"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="23">
@@ -2271,10 +2379,10 @@
       <c r="D12" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="E12" s="59" t="s">
+      <c r="E12" s="69" t="s">
         <v>24</v>
       </c>
-      <c r="F12" s="60"/>
+      <c r="F12" s="70"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="23">
@@ -2289,10 +2397,10 @@
       <c r="D13" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="E13" s="59" t="s">
+      <c r="E13" s="69" t="s">
         <v>24</v>
       </c>
-      <c r="F13" s="60"/>
+      <c r="F13" s="70"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="23">
@@ -2307,10 +2415,10 @@
       <c r="D14" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="E14" s="59" t="s">
+      <c r="E14" s="69" t="s">
         <v>24</v>
       </c>
-      <c r="F14" s="60"/>
+      <c r="F14" s="70"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="23">
@@ -2325,10 +2433,10 @@
       <c r="D15" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="E15" s="59" t="s">
+      <c r="E15" s="69" t="s">
         <v>24</v>
       </c>
-      <c r="F15" s="60"/>
+      <c r="F15" s="70"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" s="23">
@@ -2343,10 +2451,10 @@
       <c r="D16" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="E16" s="59" t="s">
+      <c r="E16" s="69" t="s">
         <v>24</v>
       </c>
-      <c r="F16" s="60"/>
+      <c r="F16" s="70"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" s="23">
@@ -2361,10 +2469,10 @@
       <c r="D17" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="E17" s="59" t="s">
+      <c r="E17" s="69" t="s">
         <v>24</v>
       </c>
-      <c r="F17" s="60"/>
+      <c r="F17" s="70"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" s="21"/>
@@ -2470,44 +2578,44 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A1" s="72" t="s">
+      <c r="A1" s="82" t="s">
         <v>40</v>
       </c>
-      <c r="B1" s="69" t="s">
+      <c r="B1" s="79" t="s">
         <v>32</v>
       </c>
-      <c r="C1" s="69" t="s">
+      <c r="C1" s="79" t="s">
         <v>33</v>
       </c>
-      <c r="D1" s="69" t="s">
+      <c r="D1" s="79" t="s">
         <v>34</v>
       </c>
-      <c r="E1" s="69" t="s">
+      <c r="E1" s="79" t="s">
         <v>35</v>
       </c>
-      <c r="F1" s="69" t="s">
+      <c r="F1" s="79" t="s">
         <v>36</v>
       </c>
-      <c r="G1" s="69" t="s">
+      <c r="G1" s="79" t="s">
         <v>37</v>
       </c>
-      <c r="H1" s="69" t="s">
+      <c r="H1" s="79" t="s">
         <v>38</v>
       </c>
-      <c r="I1" s="69" t="s">
+      <c r="I1" s="79" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A2" s="73"/>
-      <c r="B2" s="70"/>
-      <c r="C2" s="70"/>
-      <c r="D2" s="70"/>
-      <c r="E2" s="70"/>
-      <c r="F2" s="70"/>
-      <c r="G2" s="70"/>
-      <c r="H2" s="70"/>
-      <c r="I2" s="70"/>
+      <c r="A2" s="83"/>
+      <c r="B2" s="80"/>
+      <c r="C2" s="80"/>
+      <c r="D2" s="80"/>
+      <c r="E2" s="80"/>
+      <c r="F2" s="80"/>
+      <c r="G2" s="80"/>
+      <c r="H2" s="80"/>
+      <c r="I2" s="80"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
@@ -2630,17 +2738,17 @@
       </c>
     </row>
     <row r="11" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="71" t="s">
+      <c r="A11" s="81" t="s">
         <v>43</v>
       </c>
-      <c r="B11" s="71"/>
-      <c r="C11" s="71"/>
-      <c r="D11" s="71"/>
-      <c r="E11" s="71"/>
-      <c r="F11" s="71"/>
-      <c r="G11" s="71"/>
-      <c r="H11" s="71"/>
-      <c r="I11" s="71"/>
+      <c r="B11" s="81"/>
+      <c r="C11" s="81"/>
+      <c r="D11" s="81"/>
+      <c r="E11" s="81"/>
+      <c r="F11" s="81"/>
+      <c r="G11" s="81"/>
+      <c r="H11" s="81"/>
+      <c r="I11" s="81"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
@@ -2740,57 +2848,57 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="16" customFormat="1" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="74" t="s">
+      <c r="A1" s="87" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="75" t="s">
+      <c r="C1" s="84" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="75"/>
-      <c r="E1" s="75"/>
-      <c r="F1" s="75"/>
-      <c r="G1" s="75"/>
-      <c r="H1" s="75" t="s">
+      <c r="D1" s="84"/>
+      <c r="E1" s="84"/>
+      <c r="F1" s="84"/>
+      <c r="G1" s="84"/>
+      <c r="H1" s="84" t="s">
         <v>56</v>
       </c>
-      <c r="I1" s="75"/>
+      <c r="I1" s="84"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A2" s="74"/>
-      <c r="B2" s="76" t="s">
+      <c r="A2" s="87"/>
+      <c r="B2" s="85" t="s">
         <v>50</v>
       </c>
-      <c r="C2" s="75" t="s">
+      <c r="C2" s="84" t="s">
         <v>51</v>
       </c>
-      <c r="D2" s="75" t="s">
+      <c r="D2" s="84" t="s">
         <v>52</v>
       </c>
-      <c r="E2" s="74" t="s">
+      <c r="E2" s="87" t="s">
         <v>53</v>
       </c>
-      <c r="F2" s="74" t="s">
+      <c r="F2" s="87" t="s">
         <v>54</v>
       </c>
-      <c r="G2" s="75" t="s">
+      <c r="G2" s="84" t="s">
         <v>55</v>
       </c>
-      <c r="H2" s="75"/>
-      <c r="I2" s="75"/>
+      <c r="H2" s="84"/>
+      <c r="I2" s="84"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A3" s="74"/>
-      <c r="B3" s="76"/>
-      <c r="C3" s="75"/>
-      <c r="D3" s="75"/>
-      <c r="E3" s="74"/>
-      <c r="F3" s="74"/>
-      <c r="G3" s="75"/>
-      <c r="H3" s="75"/>
-      <c r="I3" s="75"/>
+      <c r="A3" s="87"/>
+      <c r="B3" s="85"/>
+      <c r="C3" s="84"/>
+      <c r="D3" s="84"/>
+      <c r="E3" s="87"/>
+      <c r="F3" s="87"/>
+      <c r="G3" s="84"/>
+      <c r="H3" s="84"/>
+      <c r="I3" s="84"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="7">
@@ -2814,10 +2922,10 @@
       <c r="G4" s="17" t="b">
         <v>1</v>
       </c>
-      <c r="H4" s="78" t="s">
+      <c r="H4" s="88" t="s">
         <v>68</v>
       </c>
-      <c r="I4" s="78"/>
+      <c r="I4" s="88"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="7">
@@ -2841,10 +2949,10 @@
       <c r="G5" s="12" t="b">
         <v>0</v>
       </c>
-      <c r="H5" s="78" t="s">
+      <c r="H5" s="88" t="s">
         <v>69</v>
       </c>
-      <c r="I5" s="78"/>
+      <c r="I5" s="88"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="7">
@@ -2868,10 +2976,10 @@
       <c r="G6" s="7" t="b">
         <v>1</v>
       </c>
-      <c r="H6" s="78" t="s">
+      <c r="H6" s="88" t="s">
         <v>70</v>
       </c>
-      <c r="I6" s="78"/>
+      <c r="I6" s="88"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="7">
@@ -2895,10 +3003,10 @@
       <c r="G7" s="7" t="b">
         <v>1</v>
       </c>
-      <c r="H7" s="78" t="s">
+      <c r="H7" s="88" t="s">
         <v>71</v>
       </c>
-      <c r="I7" s="78"/>
+      <c r="I7" s="88"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="7">
@@ -2922,10 +3030,10 @@
       <c r="G8" s="7" t="b">
         <v>1</v>
       </c>
-      <c r="H8" s="78" t="s">
+      <c r="H8" s="88" t="s">
         <v>72</v>
       </c>
-      <c r="I8" s="78"/>
+      <c r="I8" s="88"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="7">
@@ -2949,10 +3057,10 @@
       <c r="G9" s="7" t="b">
         <v>1</v>
       </c>
-      <c r="H9" s="78" t="s">
+      <c r="H9" s="88" t="s">
         <v>73</v>
       </c>
-      <c r="I9" s="78"/>
+      <c r="I9" s="88"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="7">
@@ -2976,10 +3084,10 @@
       <c r="G10" s="7" t="b">
         <v>1</v>
       </c>
-      <c r="H10" s="78" t="s">
+      <c r="H10" s="88" t="s">
         <v>74</v>
       </c>
-      <c r="I10" s="78"/>
+      <c r="I10" s="88"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="11">
@@ -3003,10 +3111,10 @@
       <c r="G11" s="14" t="b">
         <v>0</v>
       </c>
-      <c r="H11" s="77" t="s">
+      <c r="H11" s="86" t="s">
         <v>24</v>
       </c>
-      <c r="I11" s="77"/>
+      <c r="I11" s="86"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="11">
@@ -3030,10 +3138,10 @@
       <c r="G12" s="11" t="b">
         <v>1</v>
       </c>
-      <c r="H12" s="77" t="s">
+      <c r="H12" s="86" t="s">
         <v>24</v>
       </c>
-      <c r="I12" s="77"/>
+      <c r="I12" s="86"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="11">
@@ -3057,10 +3165,10 @@
       <c r="G13" s="11" t="b">
         <v>1</v>
       </c>
-      <c r="H13" s="77" t="s">
+      <c r="H13" s="86" t="s">
         <v>24</v>
       </c>
-      <c r="I13" s="77"/>
+      <c r="I13" s="86"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" s="11">
@@ -3084,10 +3192,10 @@
       <c r="G14" s="11" t="b">
         <v>1</v>
       </c>
-      <c r="H14" s="77" t="s">
+      <c r="H14" s="86" t="s">
         <v>24</v>
       </c>
-      <c r="I14" s="77"/>
+      <c r="I14" s="86"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" s="11">
@@ -3111,10 +3219,10 @@
       <c r="G15" s="11" t="b">
         <v>1</v>
       </c>
-      <c r="H15" s="77" t="s">
+      <c r="H15" s="86" t="s">
         <v>24</v>
       </c>
-      <c r="I15" s="77"/>
+      <c r="I15" s="86"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" s="11">
@@ -3138,10 +3246,10 @@
       <c r="G16" s="11" t="b">
         <v>1</v>
       </c>
-      <c r="H16" s="77" t="s">
+      <c r="H16" s="86" t="s">
         <v>24</v>
       </c>
-      <c r="I16" s="77"/>
+      <c r="I16" s="86"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" s="13" t="s">
@@ -3180,6 +3288,12 @@
     </row>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="A1:A3"/>
+    <mergeCell ref="C1:G1"/>
+    <mergeCell ref="G2:G3"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="C2:C3"/>
     <mergeCell ref="H1:I3"/>
     <mergeCell ref="B2:B3"/>
     <mergeCell ref="H16:I16"/>
@@ -3196,12 +3310,6 @@
     <mergeCell ref="H9:I9"/>
     <mergeCell ref="H8:I8"/>
     <mergeCell ref="H7:I7"/>
-    <mergeCell ref="A1:A3"/>
-    <mergeCell ref="C1:G1"/>
-    <mergeCell ref="G2:G3"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="C2:C3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
@@ -3223,40 +3331,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="72" t="s">
+      <c r="A1" s="82" t="s">
         <v>57</v>
       </c>
-      <c r="B1" s="69" t="s">
+      <c r="B1" s="79" t="s">
         <v>32</v>
       </c>
-      <c r="C1" s="69" t="s">
+      <c r="C1" s="79" t="s">
         <v>33</v>
       </c>
-      <c r="D1" s="69" t="s">
+      <c r="D1" s="79" t="s">
         <v>34</v>
       </c>
-      <c r="E1" s="69" t="s">
+      <c r="E1" s="79" t="s">
         <v>35</v>
       </c>
-      <c r="F1" s="69" t="s">
+      <c r="F1" s="79" t="s">
         <v>36</v>
       </c>
-      <c r="G1" s="69" t="s">
+      <c r="G1" s="79" t="s">
         <v>37</v>
       </c>
-      <c r="H1" s="69" t="s">
+      <c r="H1" s="79" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2" s="73"/>
-      <c r="B2" s="70"/>
-      <c r="C2" s="70"/>
-      <c r="D2" s="70"/>
-      <c r="E2" s="70"/>
-      <c r="F2" s="70"/>
-      <c r="G2" s="70"/>
-      <c r="H2" s="70"/>
+      <c r="A2" s="83"/>
+      <c r="B2" s="80"/>
+      <c r="C2" s="80"/>
+      <c r="D2" s="80"/>
+      <c r="E2" s="80"/>
+      <c r="F2" s="80"/>
+      <c r="G2" s="80"/>
+      <c r="H2" s="80"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
@@ -3357,16 +3465,16 @@
       </c>
     </row>
     <row r="10" spans="1:8" s="4" customFormat="1" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="79" t="s">
+      <c r="A10" s="89" t="s">
         <v>43</v>
       </c>
-      <c r="B10" s="79"/>
-      <c r="C10" s="79"/>
-      <c r="D10" s="79"/>
-      <c r="E10" s="79"/>
-      <c r="F10" s="79"/>
-      <c r="G10" s="79"/>
-      <c r="H10" s="79"/>
+      <c r="B10" s="89"/>
+      <c r="C10" s="89"/>
+      <c r="D10" s="89"/>
+      <c r="E10" s="89"/>
+      <c r="F10" s="89"/>
+      <c r="G10" s="89"/>
+      <c r="H10" s="89"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
@@ -3517,50 +3625,47 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44D7E2A8-7038-4E8B-9878-8235EBDD31DB}">
-  <dimension ref="A1:K45"/>
+  <dimension ref="A1:K39"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" style="21"/>
-    <col min="2" max="2" width="10.44140625" style="21" customWidth="1"/>
-    <col min="3" max="3" width="16.6640625" style="21" customWidth="1"/>
-    <col min="4" max="4" width="14.44140625" style="21" customWidth="1"/>
+    <col min="1" max="1" width="6.44140625" style="21" customWidth="1"/>
+    <col min="2" max="2" width="9.44140625" style="21" customWidth="1"/>
+    <col min="3" max="3" width="15.6640625" style="21" customWidth="1"/>
+    <col min="4" max="4" width="12.21875" style="21" customWidth="1"/>
     <col min="5" max="5" width="9.77734375" style="21" customWidth="1"/>
     <col min="6" max="6" width="8.88671875" style="28" customWidth="1"/>
     <col min="7" max="7" width="8.88671875" style="28"/>
-    <col min="8" max="16384" width="8.88671875" style="21"/>
+    <col min="8" max="8" width="15" style="29" customWidth="1"/>
+    <col min="9" max="16384" width="8.88671875" style="21"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="67" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="80" t="s">
+      <c r="A1" s="77" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="91" t="s">
         <v>96</v>
       </c>
-      <c r="C1" s="80"/>
-      <c r="D1" s="80"/>
+      <c r="C1" s="91"/>
+      <c r="D1" s="91"/>
       <c r="E1" s="18" t="s">
         <v>97</v>
       </c>
-      <c r="F1" s="80" t="s">
+      <c r="F1" s="91" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="80"/>
-      <c r="H1" s="37" t="s">
-        <v>117</v>
-      </c>
-      <c r="I1" s="41" t="s">
-        <v>136</v>
-      </c>
-      <c r="J1" s="28"/>
+      <c r="G1" s="91"/>
+      <c r="H1" s="91" t="s">
+        <v>151</v>
+      </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A2" s="67"/>
+      <c r="A2" s="77"/>
       <c r="B2" s="36" t="s">
         <v>93</v>
       </c>
@@ -3573,18 +3678,9 @@
       <c r="E2" s="18" t="s">
         <v>98</v>
       </c>
-      <c r="F2" s="80"/>
-      <c r="G2" s="80"/>
-      <c r="H2" s="21" t="s">
-        <v>135</v>
-      </c>
-      <c r="I2" s="88" t="s">
-        <v>137</v>
-      </c>
-      <c r="J2" s="88"/>
-      <c r="K2" s="21" t="s">
-        <v>141</v>
-      </c>
+      <c r="F2" s="91"/>
+      <c r="G2" s="91"/>
+      <c r="H2" s="91"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="24">
@@ -3596,25 +3692,18 @@
       <c r="C3" s="24">
         <v>1001</v>
       </c>
-      <c r="D3" s="40" t="s">
-        <v>24</v>
+      <c r="D3" s="40">
+        <v>2500</v>
       </c>
       <c r="E3" s="24" t="b">
         <v>1</v>
       </c>
-      <c r="F3" s="87" t="s">
+      <c r="F3" s="116" t="s">
         <v>106</v>
       </c>
-      <c r="G3" s="87"/>
-      <c r="H3" s="21" t="s">
-        <v>134</v>
-      </c>
-      <c r="I3" s="88" t="s">
-        <v>138</v>
-      </c>
-      <c r="J3" s="88"/>
-      <c r="K3" s="21" t="s">
-        <v>142</v>
+      <c r="G3" s="116"/>
+      <c r="H3" s="68" t="s">
+        <v>219</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
@@ -3633,17 +3722,13 @@
       <c r="E4" s="24" t="b">
         <v>1</v>
       </c>
-      <c r="F4" s="86" t="s">
+      <c r="F4" s="117" t="s">
         <v>107</v>
       </c>
-      <c r="G4" s="86"/>
-      <c r="H4" s="21" t="s">
-        <v>133</v>
-      </c>
-      <c r="I4" s="88" t="s">
-        <v>139</v>
-      </c>
-      <c r="J4" s="88"/>
+      <c r="G4" s="117"/>
+      <c r="H4" s="113" t="s">
+        <v>227</v>
+      </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="24">
@@ -3661,17 +3746,13 @@
       <c r="E5" s="24" t="b">
         <v>1</v>
       </c>
-      <c r="F5" s="85" t="s">
+      <c r="F5" s="118" t="s">
         <v>108</v>
       </c>
-      <c r="G5" s="85"/>
-      <c r="H5" s="21" t="s">
-        <v>132</v>
-      </c>
-      <c r="I5" s="88" t="s">
-        <v>140</v>
-      </c>
-      <c r="J5" s="88"/>
+      <c r="G5" s="118"/>
+      <c r="H5" s="68" t="s">
+        <v>220</v>
+      </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="24">
@@ -3684,17 +3765,18 @@
         <v>550</v>
       </c>
       <c r="D6" s="58">
-        <v>2500.0100000000002</v>
+        <v>6500.01</v>
       </c>
       <c r="E6" s="24" t="b">
         <v>0</v>
       </c>
-      <c r="F6" s="84" t="s">
+      <c r="F6" s="119" t="s">
         <v>109</v>
       </c>
-      <c r="G6" s="84"/>
-      <c r="I6" s="28"/>
-      <c r="J6" s="28"/>
+      <c r="G6" s="119"/>
+      <c r="H6" s="68" t="s">
+        <v>221</v>
+      </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="24">
@@ -3712,17 +3794,13 @@
       <c r="E7" s="24" t="b">
         <v>0</v>
       </c>
-      <c r="F7" s="81" t="s">
+      <c r="F7" s="120" t="s">
         <v>113</v>
       </c>
-      <c r="G7" s="81"/>
-      <c r="H7" s="37" t="s">
-        <v>143</v>
-      </c>
-      <c r="I7" s="41" t="s">
-        <v>144</v>
-      </c>
-      <c r="J7" s="28"/>
+      <c r="G7" s="120"/>
+      <c r="H7" s="68" t="s">
+        <v>226</v>
+      </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" s="24">
@@ -3740,19 +3818,12 @@
       <c r="E8" s="24" t="b">
         <v>0</v>
       </c>
-      <c r="F8" s="83" t="s">
+      <c r="F8" s="121" t="s">
         <v>110</v>
       </c>
-      <c r="G8" s="83"/>
-      <c r="H8" s="21" t="s">
-        <v>130</v>
-      </c>
-      <c r="I8" s="88" t="s">
-        <v>145</v>
-      </c>
-      <c r="J8" s="88"/>
-      <c r="K8" s="21" t="s">
-        <v>150</v>
+      <c r="G8" s="121"/>
+      <c r="H8" s="68" t="s">
+        <v>222</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
@@ -3771,19 +3842,12 @@
       <c r="E9" s="24" t="b">
         <v>0</v>
       </c>
-      <c r="F9" s="82" t="s">
+      <c r="F9" s="122" t="s">
         <v>111</v>
       </c>
-      <c r="G9" s="82"/>
-      <c r="H9" s="21" t="s">
-        <v>132</v>
-      </c>
-      <c r="I9" s="88" t="s">
-        <v>146</v>
-      </c>
-      <c r="J9" s="88"/>
-      <c r="K9" s="21" t="s">
-        <v>151</v>
+      <c r="G9" s="122"/>
+      <c r="H9" s="68" t="s">
+        <v>225</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
@@ -3802,17 +3866,13 @@
       <c r="E10" s="24" t="b">
         <v>0</v>
       </c>
-      <c r="F10" s="81" t="s">
+      <c r="F10" s="120" t="s">
         <v>112</v>
       </c>
-      <c r="G10" s="81"/>
-      <c r="H10" s="21" t="s">
-        <v>131</v>
-      </c>
-      <c r="I10" s="88" t="s">
-        <v>147</v>
-      </c>
-      <c r="J10" s="88"/>
+      <c r="G10" s="120"/>
+      <c r="H10" s="68" t="s">
+        <v>224</v>
+      </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" s="24">
@@ -3830,17 +3890,13 @@
       <c r="E11" s="44" t="b">
         <v>0</v>
       </c>
-      <c r="F11" s="89" t="s">
+      <c r="F11" s="123" t="s">
         <v>24</v>
       </c>
-      <c r="G11" s="89"/>
-      <c r="H11" s="21" t="s">
-        <v>133</v>
-      </c>
-      <c r="I11" s="88" t="s">
-        <v>148</v>
-      </c>
-      <c r="J11" s="88"/>
+      <c r="G11" s="123"/>
+      <c r="H11" s="67" t="s">
+        <v>228</v>
+      </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" s="24">
@@ -3858,17 +3914,13 @@
       <c r="E12" s="44" t="b">
         <v>0</v>
       </c>
-      <c r="F12" s="89" t="s">
+      <c r="F12" s="123" t="s">
         <v>24</v>
       </c>
-      <c r="G12" s="89"/>
-      <c r="H12" s="21" t="s">
-        <v>134</v>
-      </c>
-      <c r="I12" s="88" t="s">
-        <v>149</v>
-      </c>
-      <c r="J12" s="88"/>
+      <c r="G12" s="123"/>
+      <c r="H12" s="67" t="s">
+        <v>228</v>
+      </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" s="24">
@@ -3886,10 +3938,13 @@
       <c r="E13" s="44" t="b">
         <v>0</v>
       </c>
-      <c r="F13" s="89" t="s">
+      <c r="F13" s="123" t="s">
         <v>24</v>
       </c>
-      <c r="G13" s="89"/>
+      <c r="G13" s="123"/>
+      <c r="H13" s="67" t="s">
+        <v>229</v>
+      </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" s="24">
@@ -3907,349 +3962,312 @@
       <c r="E14" s="44" t="b">
         <v>0</v>
       </c>
-      <c r="F14" s="89" t="s">
+      <c r="F14" s="123" t="s">
         <v>24</v>
       </c>
-      <c r="G14" s="89"/>
+      <c r="G14" s="123"/>
+      <c r="H14" s="67" t="s">
+        <v>229</v>
+      </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" s="24">
         <v>13</v>
       </c>
-      <c r="B15" s="24"/>
+      <c r="B15" s="24" t="b">
+        <v>1</v>
+      </c>
       <c r="C15" s="24">
         <v>551</v>
       </c>
       <c r="D15" s="40">
         <v>9000.01</v>
       </c>
-      <c r="E15" s="24"/>
-      <c r="F15" s="89" t="s">
+      <c r="E15" s="24" t="b">
+        <v>1</v>
+      </c>
+      <c r="F15" s="123" t="s">
         <v>24</v>
       </c>
-      <c r="G15" s="89"/>
-      <c r="J15" s="28"/>
+      <c r="G15" s="123"/>
+      <c r="H15" s="68" t="s">
+        <v>223</v>
+      </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A16" s="24">
-        <v>14</v>
-      </c>
-      <c r="B16" s="24"/>
-      <c r="C16" s="24">
-        <v>550</v>
-      </c>
-      <c r="D16" s="40">
-        <v>6500.01</v>
-      </c>
-      <c r="E16" s="24"/>
-      <c r="F16" s="89" t="s">
-        <v>24</v>
-      </c>
-      <c r="G16" s="89"/>
-      <c r="J16" s="28"/>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A17" s="24">
-        <v>15</v>
-      </c>
-      <c r="B17" s="24"/>
-      <c r="C17" s="24">
-        <v>1000</v>
-      </c>
-      <c r="D17" s="40">
-        <v>2499.9899999999998</v>
-      </c>
-      <c r="E17" s="24"/>
-      <c r="F17" s="89" t="s">
-        <v>24</v>
-      </c>
-      <c r="G17" s="89"/>
-      <c r="J17" s="28"/>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A18" s="24">
-        <v>16</v>
-      </c>
-      <c r="B18" s="24"/>
-      <c r="C18" s="24">
-        <v>1001</v>
-      </c>
-      <c r="D18" s="40">
-        <v>6500.01</v>
-      </c>
-      <c r="E18" s="24"/>
-      <c r="F18" s="89" t="s">
-        <v>24</v>
-      </c>
-      <c r="G18" s="89"/>
-      <c r="J18" s="28"/>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A19" s="24">
-        <v>17</v>
-      </c>
-      <c r="B19" s="24"/>
-      <c r="C19" s="24">
-        <v>1001</v>
-      </c>
-      <c r="D19" s="40">
-        <v>2499.9899999999998</v>
-      </c>
-      <c r="E19" s="24"/>
-      <c r="F19" s="89" t="s">
-        <v>24</v>
-      </c>
-      <c r="G19" s="89"/>
-      <c r="J19" s="28"/>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A20" s="29"/>
-      <c r="B20" s="29"/>
-      <c r="C20" s="29"/>
-      <c r="D20" s="39"/>
-      <c r="E20" s="29"/>
-      <c r="J20" s="28"/>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A21" s="29"/>
-      <c r="B21" s="29"/>
-      <c r="C21" s="29"/>
-      <c r="D21" s="39"/>
-      <c r="E21" s="29"/>
-      <c r="J21" s="28"/>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="J22" s="28"/>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A23" s="37" t="s">
+      <c r="A16" s="29"/>
+      <c r="B16" s="29"/>
+      <c r="C16" s="29"/>
+      <c r="D16" s="39"/>
+      <c r="E16" s="29"/>
+      <c r="H16" s="110"/>
+      <c r="K16" s="28"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A17" s="29"/>
+      <c r="B17" s="29"/>
+      <c r="C17" s="29"/>
+      <c r="D17" s="39"/>
+      <c r="E17" s="29"/>
+      <c r="H17" s="110"/>
+      <c r="K17" s="28"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="H18" s="110"/>
+      <c r="K18" s="28"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A19" s="37" t="s">
         <v>99</v>
       </c>
-      <c r="B23" s="21" t="s">
+      <c r="B19" s="21" t="s">
         <v>102</v>
       </c>
-      <c r="C23" s="21" t="s">
+      <c r="C19" s="21" t="s">
         <v>101</v>
       </c>
-      <c r="D23" s="21" t="s">
+      <c r="D19" s="21" t="s">
         <v>114</v>
       </c>
-      <c r="E23" s="21" t="s">
+      <c r="E19" s="21" t="s">
         <v>103</v>
       </c>
-      <c r="J23" s="28"/>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A24" s="37" t="s">
+      <c r="H19" s="110"/>
+      <c r="K19" s="28"/>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A20" s="37" t="s">
         <v>100</v>
       </c>
+      <c r="B20" s="21" t="s">
+        <v>104</v>
+      </c>
+      <c r="C20" s="21" t="s">
+        <v>105</v>
+      </c>
+      <c r="D20" s="21" t="s">
+        <v>115</v>
+      </c>
+      <c r="K20" s="28"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="K21" s="28"/>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A22" s="21" t="s">
+        <v>116</v>
+      </c>
+      <c r="K22" s="28"/>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B23" s="37" t="s">
+        <v>141</v>
+      </c>
+      <c r="E23" s="37"/>
+      <c r="F23" s="41"/>
+      <c r="K23" s="28"/>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B24" s="21" t="s">
-        <v>104</v>
+        <v>118</v>
       </c>
       <c r="C24" s="21" t="s">
-        <v>105</v>
-      </c>
-      <c r="D24" s="21" t="s">
-        <v>115</v>
-      </c>
-      <c r="I24" s="28"/>
+        <v>119</v>
+      </c>
+      <c r="D24" s="37" t="s">
+        <v>117</v>
+      </c>
+      <c r="E24" s="41" t="s">
+        <v>136</v>
+      </c>
+      <c r="G24" s="21"/>
       <c r="J24" s="28"/>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A27" s="21" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B29" s="37" t="s">
+      <c r="K24" s="28"/>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B25" s="21" t="s">
+        <v>120</v>
+      </c>
+      <c r="C25" s="21" t="s">
+        <v>121</v>
+      </c>
+      <c r="D25" s="21" t="s">
+        <v>135</v>
+      </c>
+      <c r="E25" s="90" t="s">
+        <v>137</v>
+      </c>
+      <c r="F25" s="90"/>
+      <c r="G25" s="21" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B26" s="21" t="s">
+        <v>122</v>
+      </c>
+      <c r="C26" s="21" t="s">
+        <v>123</v>
+      </c>
+      <c r="D26" s="21" t="s">
+        <v>134</v>
+      </c>
+      <c r="E26" s="90" t="s">
+        <v>212</v>
+      </c>
+      <c r="F26" s="90"/>
+      <c r="G26" s="21" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B27" s="21" t="s">
+        <v>124</v>
+      </c>
+      <c r="C27" s="21" t="s">
+        <v>125</v>
+      </c>
+      <c r="D27" s="21" t="s">
+        <v>133</v>
+      </c>
+      <c r="E27" s="90" t="s">
+        <v>213</v>
+      </c>
+      <c r="F27" s="90"/>
+      <c r="G27" s="21" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B28" s="21" t="s">
+        <v>126</v>
+      </c>
+      <c r="C28" s="21" t="s">
+        <v>127</v>
+      </c>
+      <c r="D28" s="21" t="s">
+        <v>132</v>
+      </c>
+      <c r="E28" s="90" t="s">
+        <v>138</v>
+      </c>
+      <c r="F28" s="90"/>
+      <c r="G28" s="21" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B29" s="21" t="s">
+        <v>128</v>
+      </c>
+      <c r="C29" s="21" t="s">
+        <v>129</v>
+      </c>
+      <c r="E29" s="28"/>
+      <c r="G29" s="21"/>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="D30" s="37" t="s">
+        <v>141</v>
+      </c>
+      <c r="E30" s="41" t="s">
+        <v>142</v>
+      </c>
+      <c r="G30" s="21"/>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B31" s="21" t="s">
+        <v>230</v>
+      </c>
+      <c r="D31" s="21" t="s">
+        <v>130</v>
+      </c>
+      <c r="E31" s="90" t="s">
         <v>143</v>
       </c>
-      <c r="E29" s="37" t="s">
-        <v>117</v>
-      </c>
-      <c r="F29" s="41" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B30" s="21" t="s">
+      <c r="F31" s="90"/>
+      <c r="G31" s="21" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B32" s="21" t="s">
         <v>118</v>
       </c>
-      <c r="C30" s="21" t="s">
-        <v>119</v>
-      </c>
-      <c r="E30" s="21" t="s">
-        <v>135</v>
-      </c>
-      <c r="F30" s="88" t="s">
-        <v>137</v>
-      </c>
-      <c r="G30" s="88"/>
-      <c r="H30" s="21" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B31" s="21" t="s">
+      <c r="C32" s="21" t="s">
+        <v>231</v>
+      </c>
+      <c r="D32" s="21" t="s">
+        <v>132</v>
+      </c>
+      <c r="E32" s="90" t="s">
+        <v>144</v>
+      </c>
+      <c r="F32" s="90"/>
+      <c r="G32" s="21" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="33" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B33" s="21" t="s">
         <v>120</v>
       </c>
-      <c r="C31" s="21" t="s">
-        <v>121</v>
-      </c>
-      <c r="E31" s="21" t="s">
+      <c r="C33" s="21" t="s">
+        <v>233</v>
+      </c>
+      <c r="D33" s="21" t="s">
+        <v>131</v>
+      </c>
+      <c r="E33" s="90" t="s">
+        <v>214</v>
+      </c>
+      <c r="F33" s="90"/>
+      <c r="G33" s="21" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="34" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B34" s="21" t="s">
+        <v>232</v>
+      </c>
+      <c r="D34" s="21" t="s">
+        <v>133</v>
+      </c>
+      <c r="E34" s="90" t="s">
+        <v>145</v>
+      </c>
+      <c r="F34" s="90"/>
+      <c r="G34" s="21"/>
+    </row>
+    <row r="35" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="D35" s="21" t="s">
         <v>134</v>
       </c>
-      <c r="F31" s="88" t="s">
-        <v>138</v>
-      </c>
-      <c r="G31" s="88"/>
-      <c r="H31" s="21" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B32" s="21" t="s">
-        <v>122</v>
-      </c>
-      <c r="C32" s="21" t="s">
-        <v>123</v>
-      </c>
-      <c r="E32" s="21" t="s">
-        <v>133</v>
-      </c>
-      <c r="F32" s="88" t="s">
-        <v>139</v>
-      </c>
-      <c r="G32" s="88"/>
-    </row>
-    <row r="33" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B33" s="21" t="s">
-        <v>124</v>
-      </c>
-      <c r="C33" s="21" t="s">
-        <v>125</v>
-      </c>
-      <c r="E33" s="21" t="s">
-        <v>132</v>
-      </c>
-      <c r="F33" s="88" t="s">
-        <v>140</v>
-      </c>
-      <c r="G33" s="88"/>
-    </row>
-    <row r="34" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B34" s="21" t="s">
-        <v>126</v>
-      </c>
-      <c r="C34" s="21" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="35" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B35" s="21" t="s">
-        <v>128</v>
-      </c>
-      <c r="C35" s="21" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="37" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="E37" s="37" t="s">
-        <v>143</v>
-      </c>
-      <c r="F37" s="41" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="38" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="E38" s="21" t="s">
-        <v>130</v>
-      </c>
-      <c r="F38" s="88" t="s">
-        <v>145</v>
-      </c>
-      <c r="G38" s="88"/>
-      <c r="H38" s="21" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="39" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="E39" s="21" t="s">
-        <v>132</v>
-      </c>
-      <c r="F39" s="88" t="s">
-        <v>146</v>
-      </c>
-      <c r="G39" s="88"/>
-      <c r="H39" s="21" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="40" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="E40" s="21" t="s">
-        <v>131</v>
-      </c>
-      <c r="F40" s="88" t="s">
-        <v>147</v>
-      </c>
-      <c r="G40" s="88"/>
-    </row>
-    <row r="41" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="E41" s="21" t="s">
-        <v>133</v>
-      </c>
-      <c r="F41" s="88" t="s">
-        <v>148</v>
-      </c>
-      <c r="G41" s="88"/>
-    </row>
-    <row r="42" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="E42" s="21" t="s">
-        <v>134</v>
-      </c>
-      <c r="F42" s="88" t="s">
-        <v>149</v>
-      </c>
-      <c r="G42" s="88"/>
-    </row>
-    <row r="43" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="F43" s="21"/>
-    </row>
-    <row r="44" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="F44" s="21"/>
-    </row>
-    <row r="45" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="F45" s="21"/>
+      <c r="E35" s="90" t="s">
+        <v>211</v>
+      </c>
+      <c r="F35" s="90"/>
+      <c r="G35" s="21" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="36" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="F36" s="21"/>
+      <c r="G36" s="21"/>
+    </row>
+    <row r="37" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="F37" s="21"/>
+      <c r="G37" s="21"/>
+    </row>
+    <row r="38" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="G38" s="21"/>
+    </row>
+    <row r="39" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="F39" s="21"/>
     </row>
   </sheetData>
-  <mergeCells count="38">
-    <mergeCell ref="I9:J9"/>
-    <mergeCell ref="I10:J10"/>
-    <mergeCell ref="I11:J11"/>
-    <mergeCell ref="I12:J12"/>
-    <mergeCell ref="F11:G11"/>
-    <mergeCell ref="F12:G12"/>
-    <mergeCell ref="F42:G42"/>
-    <mergeCell ref="F41:G41"/>
-    <mergeCell ref="F40:G40"/>
-    <mergeCell ref="F39:G39"/>
-    <mergeCell ref="F38:G38"/>
-    <mergeCell ref="I2:J2"/>
-    <mergeCell ref="I3:J3"/>
-    <mergeCell ref="I4:J4"/>
-    <mergeCell ref="I5:J5"/>
-    <mergeCell ref="I8:J8"/>
-    <mergeCell ref="F33:G33"/>
-    <mergeCell ref="F32:G32"/>
-    <mergeCell ref="F31:G31"/>
-    <mergeCell ref="F30:G30"/>
-    <mergeCell ref="F13:G13"/>
-    <mergeCell ref="F14:G14"/>
-    <mergeCell ref="F15:G15"/>
-    <mergeCell ref="F16:G16"/>
-    <mergeCell ref="F17:G17"/>
-    <mergeCell ref="F18:G18"/>
-    <mergeCell ref="F19:G19"/>
+  <mergeCells count="26">
+    <mergeCell ref="H1:H2"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:D1"/>
     <mergeCell ref="F1:G2"/>
@@ -4261,6 +4279,20 @@
     <mergeCell ref="F4:G4"/>
     <mergeCell ref="F3:G3"/>
     <mergeCell ref="F7:G7"/>
+    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="F15:G15"/>
+    <mergeCell ref="E25:F25"/>
+    <mergeCell ref="E26:F26"/>
+    <mergeCell ref="E27:F27"/>
+    <mergeCell ref="E28:F28"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="F12:G12"/>
   </mergeCells>
   <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4271,10 +4303,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCF6D9F7-D4E3-49EA-A4E4-B61C1736EDE1}">
-  <dimension ref="A1:J30"/>
+  <dimension ref="A1:J32"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView zoomScale="93" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4282,64 +4314,64 @@
     <col min="1" max="1" width="9.88671875" customWidth="1"/>
     <col min="2" max="2" width="10.6640625" customWidth="1"/>
     <col min="3" max="3" width="12.88671875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="10.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.88671875" style="1" customWidth="1"/>
     <col min="5" max="5" width="16.33203125" customWidth="1"/>
     <col min="7" max="7" width="12" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="67" t="s">
-        <v>169</v>
-      </c>
-      <c r="B1" s="68" t="s">
+      <c r="A1" s="77" t="s">
+        <v>165</v>
+      </c>
+      <c r="B1" s="78" t="s">
         <v>96</v>
       </c>
-      <c r="C1" s="68"/>
-      <c r="D1" s="68"/>
+      <c r="C1" s="78"/>
+      <c r="D1" s="78"/>
       <c r="E1" s="20" t="s">
         <v>97</v>
       </c>
-      <c r="F1" s="67" t="s">
+      <c r="F1" s="77" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="67"/>
-      <c r="H1" s="80" t="s">
-        <v>155</v>
-      </c>
-      <c r="I1" s="80"/>
-      <c r="J1" s="80"/>
+      <c r="G1" s="77"/>
+      <c r="H1" s="91" t="s">
+        <v>151</v>
+      </c>
+      <c r="I1" s="91"/>
+      <c r="J1" s="91"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A2" s="67"/>
-      <c r="B2" s="67" t="s">
-        <v>152</v>
-      </c>
-      <c r="C2" s="92" t="s">
-        <v>153</v>
-      </c>
-      <c r="D2" s="67" t="s">
-        <v>154</v>
-      </c>
-      <c r="E2" s="80" t="s">
-        <v>170</v>
-      </c>
-      <c r="F2" s="67"/>
-      <c r="G2" s="67"/>
-      <c r="H2" s="80"/>
-      <c r="I2" s="80"/>
-      <c r="J2" s="80"/>
+      <c r="A2" s="77"/>
+      <c r="B2" s="77" t="s">
+        <v>148</v>
+      </c>
+      <c r="C2" s="99" t="s">
+        <v>149</v>
+      </c>
+      <c r="D2" s="77" t="s">
+        <v>150</v>
+      </c>
+      <c r="E2" s="91" t="s">
+        <v>166</v>
+      </c>
+      <c r="F2" s="77"/>
+      <c r="G2" s="77"/>
+      <c r="H2" s="91"/>
+      <c r="I2" s="91"/>
+      <c r="J2" s="91"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A3" s="67"/>
-      <c r="B3" s="67"/>
-      <c r="C3" s="92"/>
-      <c r="D3" s="67"/>
-      <c r="E3" s="80"/>
-      <c r="F3" s="67"/>
-      <c r="G3" s="67"/>
-      <c r="H3" s="80"/>
-      <c r="I3" s="80"/>
-      <c r="J3" s="80"/>
+      <c r="A3" s="77"/>
+      <c r="B3" s="77"/>
+      <c r="C3" s="99"/>
+      <c r="D3" s="77"/>
+      <c r="E3" s="91"/>
+      <c r="F3" s="77"/>
+      <c r="G3" s="77"/>
+      <c r="H3" s="91"/>
+      <c r="I3" s="91"/>
+      <c r="J3" s="91"/>
     </row>
     <row r="4" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="24">
@@ -4355,15 +4387,15 @@
         <v>4999.8999999999996</v>
       </c>
       <c r="E4" s="49" t="s">
-        <v>164</v>
-      </c>
-      <c r="F4" s="93" t="s">
-        <v>156</v>
-      </c>
-      <c r="G4" s="93"/>
-      <c r="H4" s="91"/>
-      <c r="I4" s="91"/>
-      <c r="J4" s="91"/>
+        <v>160</v>
+      </c>
+      <c r="F4" s="96" t="s">
+        <v>152</v>
+      </c>
+      <c r="G4" s="96"/>
+      <c r="H4" s="95"/>
+      <c r="I4" s="95"/>
+      <c r="J4" s="95"/>
     </row>
     <row r="5" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A5" s="24">
@@ -4372,22 +4404,22 @@
       <c r="B5" s="46" t="b">
         <v>0</v>
       </c>
-      <c r="C5" s="47">
+      <c r="C5" s="114">
         <v>212.1</v>
       </c>
-      <c r="D5" s="48">
+      <c r="D5" s="115">
         <v>4999.8999999999996</v>
       </c>
       <c r="E5" s="49" t="s">
-        <v>165</v>
-      </c>
-      <c r="F5" s="94" t="s">
-        <v>157</v>
-      </c>
-      <c r="G5" s="94"/>
-      <c r="H5" s="91"/>
-      <c r="I5" s="91"/>
-      <c r="J5" s="91"/>
+        <v>161</v>
+      </c>
+      <c r="F5" s="97" t="s">
+        <v>153</v>
+      </c>
+      <c r="G5" s="97"/>
+      <c r="H5" s="95"/>
+      <c r="I5" s="95"/>
+      <c r="J5" s="95"/>
     </row>
     <row r="6" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A6" s="24">
@@ -4403,15 +4435,15 @@
         <v>3499.9</v>
       </c>
       <c r="E6" s="49" t="s">
-        <v>166</v>
-      </c>
-      <c r="F6" s="95" t="s">
-        <v>158</v>
-      </c>
-      <c r="G6" s="95"/>
-      <c r="H6" s="91"/>
-      <c r="I6" s="91"/>
-      <c r="J6" s="91"/>
+        <v>162</v>
+      </c>
+      <c r="F6" s="98" t="s">
+        <v>154</v>
+      </c>
+      <c r="G6" s="98"/>
+      <c r="H6" s="95"/>
+      <c r="I6" s="95"/>
+      <c r="J6" s="95"/>
     </row>
     <row r="7" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A7" s="24">
@@ -4427,15 +4459,15 @@
         <v>3499.9</v>
       </c>
       <c r="E7" s="49" t="s">
-        <v>167</v>
-      </c>
-      <c r="F7" s="90" t="s">
-        <v>159</v>
-      </c>
-      <c r="G7" s="90"/>
-      <c r="H7" s="91"/>
-      <c r="I7" s="91"/>
-      <c r="J7" s="91"/>
+        <v>163</v>
+      </c>
+      <c r="F7" s="94" t="s">
+        <v>155</v>
+      </c>
+      <c r="G7" s="94"/>
+      <c r="H7" s="95"/>
+      <c r="I7" s="95"/>
+      <c r="J7" s="95"/>
     </row>
     <row r="8" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A8" s="24">
@@ -4451,15 +4483,15 @@
         <v>3499.9</v>
       </c>
       <c r="E8" s="49" t="s">
-        <v>167</v>
-      </c>
-      <c r="F8" s="90" t="s">
-        <v>160</v>
-      </c>
-      <c r="G8" s="90"/>
-      <c r="H8" s="91"/>
-      <c r="I8" s="91"/>
-      <c r="J8" s="91"/>
+        <v>163</v>
+      </c>
+      <c r="F8" s="94" t="s">
+        <v>156</v>
+      </c>
+      <c r="G8" s="94"/>
+      <c r="H8" s="95"/>
+      <c r="I8" s="95"/>
+      <c r="J8" s="95"/>
     </row>
     <row r="9" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A9" s="24">
@@ -4475,15 +4507,15 @@
         <v>5000</v>
       </c>
       <c r="E9" s="49" t="s">
-        <v>167</v>
-      </c>
-      <c r="F9" s="90" t="s">
-        <v>161</v>
-      </c>
-      <c r="G9" s="90"/>
-      <c r="H9" s="91"/>
-      <c r="I9" s="91"/>
-      <c r="J9" s="91"/>
+        <v>163</v>
+      </c>
+      <c r="F9" s="94" t="s">
+        <v>157</v>
+      </c>
+      <c r="G9" s="94"/>
+      <c r="H9" s="95"/>
+      <c r="I9" s="95"/>
+      <c r="J9" s="95"/>
     </row>
     <row r="10" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A10" s="24">
@@ -4499,15 +4531,15 @@
         <v>1900</v>
       </c>
       <c r="E10" s="49" t="s">
-        <v>167</v>
-      </c>
-      <c r="F10" s="90" t="s">
-        <v>162</v>
-      </c>
-      <c r="G10" s="90"/>
-      <c r="H10" s="91"/>
-      <c r="I10" s="91"/>
-      <c r="J10" s="91"/>
+        <v>163</v>
+      </c>
+      <c r="F10" s="94" t="s">
+        <v>158</v>
+      </c>
+      <c r="G10" s="94"/>
+      <c r="H10" s="95"/>
+      <c r="I10" s="95"/>
+      <c r="J10" s="95"/>
     </row>
     <row r="11" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A11" s="24">
@@ -4523,15 +4555,15 @@
         <v>3500</v>
       </c>
       <c r="E11" s="49" t="s">
-        <v>167</v>
-      </c>
-      <c r="F11" s="90" t="s">
         <v>163</v>
       </c>
-      <c r="G11" s="90"/>
-      <c r="H11" s="91"/>
-      <c r="I11" s="91"/>
-      <c r="J11" s="91"/>
+      <c r="F11" s="94" t="s">
+        <v>159</v>
+      </c>
+      <c r="G11" s="94"/>
+      <c r="H11" s="95"/>
+      <c r="I11" s="95"/>
+      <c r="J11" s="95"/>
     </row>
     <row r="12" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A12" s="24">
@@ -4547,15 +4579,15 @@
         <v>3500</v>
       </c>
       <c r="E12" s="57" t="s">
-        <v>167</v>
-      </c>
-      <c r="F12" s="90" t="s">
-        <v>24</v>
-      </c>
-      <c r="G12" s="90"/>
-      <c r="H12" s="91"/>
-      <c r="I12" s="91"/>
-      <c r="J12" s="91"/>
+        <v>163</v>
+      </c>
+      <c r="F12" s="94" t="s">
+        <v>234</v>
+      </c>
+      <c r="G12" s="94"/>
+      <c r="H12" s="95"/>
+      <c r="I12" s="95"/>
+      <c r="J12" s="95"/>
     </row>
     <row r="13" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A13" s="24">
@@ -4571,15 +4603,15 @@
         <v>3500</v>
       </c>
       <c r="E13" s="57" t="s">
-        <v>167</v>
-      </c>
-      <c r="F13" s="90" t="s">
-        <v>24</v>
-      </c>
-      <c r="G13" s="90"/>
-      <c r="H13" s="91"/>
-      <c r="I13" s="91"/>
-      <c r="J13" s="91"/>
+        <v>163</v>
+      </c>
+      <c r="F13" s="94" t="s">
+        <v>234</v>
+      </c>
+      <c r="G13" s="94"/>
+      <c r="H13" s="95"/>
+      <c r="I13" s="95"/>
+      <c r="J13" s="95"/>
     </row>
     <row r="14" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A14" s="24">
@@ -4592,18 +4624,18 @@
         <v>100</v>
       </c>
       <c r="D14" s="54" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="E14" s="57" t="s">
-        <v>167</v>
-      </c>
-      <c r="F14" s="90" t="s">
+        <v>163</v>
+      </c>
+      <c r="F14" s="94" t="s">
         <v>24</v>
       </c>
-      <c r="G14" s="90"/>
-      <c r="H14" s="91"/>
-      <c r="I14" s="91"/>
-      <c r="J14" s="91"/>
+      <c r="G14" s="94"/>
+      <c r="H14" s="95"/>
+      <c r="I14" s="95"/>
+      <c r="J14" s="95"/>
     </row>
     <row r="15" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A15" s="24">
@@ -4619,184 +4651,187 @@
         <v>10000</v>
       </c>
       <c r="E15" s="57" t="s">
+        <v>163</v>
+      </c>
+      <c r="F15" s="94" t="s">
+        <v>24</v>
+      </c>
+      <c r="G15" s="94"/>
+      <c r="H15" s="95"/>
+      <c r="I15" s="95"/>
+      <c r="J15" s="95"/>
+    </row>
+    <row r="16" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A16" s="110"/>
+      <c r="C16"/>
+      <c r="D16"/>
+      <c r="G16" s="111"/>
+      <c r="H16" s="112"/>
+      <c r="I16" s="112"/>
+      <c r="J16" s="112"/>
+    </row>
+    <row r="17" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A17" s="110"/>
+      <c r="C17"/>
+      <c r="D17"/>
+      <c r="G17" s="111"/>
+      <c r="H17" s="112"/>
+      <c r="I17" s="112"/>
+      <c r="J17" s="112"/>
+    </row>
+    <row r="18" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="C18"/>
+      <c r="D18"/>
+      <c r="G18" s="111"/>
+      <c r="H18" s="112"/>
+      <c r="I18" s="112"/>
+      <c r="J18" s="112"/>
+    </row>
+    <row r="19" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="C19" s="42"/>
+      <c r="D19" s="43"/>
+      <c r="F19" s="111"/>
+      <c r="G19" s="111"/>
+      <c r="H19" s="112"/>
+      <c r="I19" s="112"/>
+      <c r="J19" s="112"/>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A20" s="35" t="s">
         <v>167</v>
       </c>
-      <c r="F15" s="90" t="s">
-        <v>24</v>
-      </c>
-      <c r="G15" s="90"/>
-      <c r="H15" s="91"/>
-      <c r="I15" s="91"/>
-      <c r="J15" s="91"/>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="C16" s="42"/>
-      <c r="D16" s="43"/>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C17" s="42"/>
-      <c r="D17" s="43"/>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A18" s="35" t="s">
+      <c r="B20" s="35" t="s">
+        <v>179</v>
+      </c>
+      <c r="C20" s="42"/>
+      <c r="D20" s="43"/>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>168</v>
+      </c>
+      <c r="B21" s="92" t="s">
+        <v>174</v>
+      </c>
+      <c r="C21" s="92"/>
+      <c r="D21" s="43" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>169</v>
+      </c>
+      <c r="B22" s="92" t="s">
+        <v>173</v>
+      </c>
+      <c r="C22" s="92"/>
+      <c r="D22" s="43" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>170</v>
+      </c>
+      <c r="B23" s="92" t="s">
+        <v>175</v>
+      </c>
+      <c r="C23" s="92"/>
+      <c r="D23" s="43" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A24" s="56" t="s">
         <v>171</v>
       </c>
-      <c r="B18" s="35" t="s">
+      <c r="B24" s="93" t="s">
+        <v>176</v>
+      </c>
+      <c r="C24" s="93"/>
+      <c r="D24" s="43"/>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A25" s="56" t="s">
+        <v>172</v>
+      </c>
+      <c r="B25" s="93" t="s">
+        <v>177</v>
+      </c>
+      <c r="C25" s="93"/>
+      <c r="D25" s="43"/>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A27" s="35" t="s">
+        <v>167</v>
+      </c>
+      <c r="B27" s="35" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>168</v>
+      </c>
+      <c r="B28" s="92" t="s">
+        <v>180</v>
+      </c>
+      <c r="C28" s="92"/>
+      <c r="D28" s="1" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>169</v>
+      </c>
+      <c r="B29" s="92" t="s">
+        <v>182</v>
+      </c>
+      <c r="C29" s="92"/>
+      <c r="D29" s="1" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>170</v>
+      </c>
+      <c r="B30" s="92" t="s">
+        <v>181</v>
+      </c>
+      <c r="C30" s="92"/>
+      <c r="D30" s="1" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>171</v>
+      </c>
+      <c r="B31" s="92" t="s">
         <v>183</v>
       </c>
-      <c r="C18" s="42"/>
-      <c r="D18" s="43"/>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
+      <c r="C31" s="92"/>
+      <c r="D31" s="1" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
         <v>172</v>
       </c>
-      <c r="B19" s="96" t="s">
-        <v>178</v>
-      </c>
-      <c r="C19" s="96"/>
-      <c r="D19" s="43" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
-        <v>173</v>
-      </c>
-      <c r="B20" s="96" t="s">
-        <v>177</v>
-      </c>
-      <c r="C20" s="96"/>
-      <c r="D20" s="43" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
-        <v>174</v>
-      </c>
-      <c r="B21" s="96" t="s">
-        <v>179</v>
-      </c>
-      <c r="C21" s="96"/>
-      <c r="D21" s="43"/>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A22" s="56" t="s">
-        <v>175</v>
-      </c>
-      <c r="B22" s="97" t="s">
-        <v>180</v>
-      </c>
-      <c r="C22" s="97"/>
-      <c r="D22" s="43"/>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A23" s="56" t="s">
-        <v>176</v>
-      </c>
-      <c r="B23" s="97" t="s">
-        <v>181</v>
-      </c>
-      <c r="C23" s="97"/>
-      <c r="D23" s="43"/>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A25" s="35" t="s">
-        <v>171</v>
-      </c>
-      <c r="B25" s="35" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
-        <v>172</v>
-      </c>
-      <c r="B26" s="96" t="s">
+      <c r="B32" s="92" t="s">
         <v>184</v>
       </c>
-      <c r="C26" s="96"/>
-      <c r="D26" s="1" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
-        <v>173</v>
-      </c>
-      <c r="B27" s="96" t="s">
-        <v>186</v>
-      </c>
-      <c r="C27" s="96"/>
-      <c r="D27" s="1" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
-        <v>174</v>
-      </c>
-      <c r="B28" s="96" t="s">
-        <v>185</v>
-      </c>
-      <c r="C28" s="96"/>
-      <c r="D28" s="1" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
-        <v>175</v>
-      </c>
-      <c r="B29" s="96" t="s">
-        <v>187</v>
-      </c>
-      <c r="C29" s="96"/>
-      <c r="D29" s="1" t="s">
+      <c r="C32" s="92"/>
+      <c r="D32" s="1" t="s">
         <v>189</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A30" t="s">
-        <v>176</v>
-      </c>
-      <c r="B30" s="96" t="s">
-        <v>188</v>
-      </c>
-      <c r="C30" s="96"/>
-      <c r="D30" s="1" t="s">
-        <v>193</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="42">
-    <mergeCell ref="B28:C28"/>
-    <mergeCell ref="B29:C29"/>
-    <mergeCell ref="B30:C30"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="F9:G9"/>
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="F11:G11"/>
-    <mergeCell ref="H12:J12"/>
-    <mergeCell ref="H13:J13"/>
-    <mergeCell ref="H14:J14"/>
-    <mergeCell ref="H15:J15"/>
-    <mergeCell ref="F12:G12"/>
-    <mergeCell ref="F13:G13"/>
-    <mergeCell ref="F14:G14"/>
-    <mergeCell ref="F15:G15"/>
-    <mergeCell ref="H4:J4"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="F5:G5"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="F7:G7"/>
     <mergeCell ref="F8:G8"/>
     <mergeCell ref="F1:G3"/>
     <mergeCell ref="H1:J3"/>
@@ -4813,28 +4848,54 @@
     <mergeCell ref="D2:D3"/>
     <mergeCell ref="E2:E3"/>
     <mergeCell ref="B1:D1"/>
+    <mergeCell ref="H4:J4"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="F9:G9"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="H12:J12"/>
+    <mergeCell ref="H13:J13"/>
+    <mergeCell ref="H14:J14"/>
+    <mergeCell ref="H15:J15"/>
+    <mergeCell ref="F12:G12"/>
+    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="F15:G15"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="B29:C29"/>
   </mergeCells>
   <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="landscape" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83FABE2F-9C9C-4A9F-9234-D36F5EBE9127}">
-  <dimension ref="A1:N13"/>
+  <dimension ref="A1:Q22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L7" sqref="L7"/>
+    <sheetView tabSelected="1" zoomScale="134" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14:E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" style="100"/>
-    <col min="2" max="3" width="8.88671875" style="102"/>
-    <col min="4" max="4" width="10.109375" style="99" customWidth="1"/>
-    <col min="5" max="5" width="11.44140625" style="99" customWidth="1"/>
+    <col min="1" max="1" width="8.88671875" style="61"/>
+    <col min="2" max="3" width="8.88671875" style="63"/>
+    <col min="4" max="4" width="10.109375" style="125" customWidth="1"/>
+    <col min="5" max="5" width="11.44140625" style="60" customWidth="1"/>
     <col min="8" max="8" width="11.33203125" customWidth="1"/>
     <col min="9" max="9" width="11.5546875" customWidth="1"/>
     <col min="10" max="10" width="9.21875" customWidth="1"/>
@@ -4843,245 +4904,406 @@
     <col min="14" max="14" width="10.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="74" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="101" t="s">
+    <row r="1" spans="1:17" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="87" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="62" t="s">
         <v>96</v>
       </c>
-      <c r="C1" s="101" t="s">
-        <v>196</v>
-      </c>
-      <c r="D1" s="74" t="s">
+      <c r="C1" s="62" t="s">
+        <v>192</v>
+      </c>
+      <c r="D1" s="87" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="74"/>
-    </row>
-    <row r="2" spans="1:14" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="74"/>
-      <c r="B2" s="101" t="s">
-        <v>197</v>
-      </c>
-      <c r="C2" s="101" t="s">
-        <v>198</v>
-      </c>
-      <c r="D2" s="74"/>
-      <c r="E2" s="74"/>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A3" s="103">
-        <v>1</v>
-      </c>
-      <c r="B3" s="104" t="s">
-        <v>206</v>
-      </c>
-      <c r="C3" s="105">
+      <c r="E1" s="87"/>
+    </row>
+    <row r="2" spans="1:17" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="87"/>
+      <c r="B2" s="62" t="s">
+        <v>193</v>
+      </c>
+      <c r="C2" s="62" t="s">
+        <v>194</v>
+      </c>
+      <c r="D2" s="87"/>
+      <c r="E2" s="87"/>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A3" s="64">
+        <v>1</v>
+      </c>
+      <c r="B3" s="65" t="s">
+        <v>202</v>
+      </c>
+      <c r="C3" s="66">
         <v>6</v>
       </c>
-      <c r="D3" s="106" t="s">
-        <v>207</v>
-      </c>
-      <c r="E3" s="107"/>
+      <c r="D3" s="100" t="s">
+        <v>203</v>
+      </c>
+      <c r="E3" s="101"/>
       <c r="G3" t="s">
         <v>7</v>
       </c>
-      <c r="H3" s="98" t="s">
+      <c r="H3" s="59" t="s">
+        <v>195</v>
+      </c>
+      <c r="I3" s="59" t="s">
+        <v>196</v>
+      </c>
+      <c r="J3" t="s">
+        <v>197</v>
+      </c>
+      <c r="K3" t="s">
+        <v>198</v>
+      </c>
+      <c r="L3" t="s">
         <v>199</v>
       </c>
-      <c r="I3" s="98" t="s">
+      <c r="M3" t="s">
         <v>200</v>
       </c>
-      <c r="J3" t="s">
+      <c r="N3" t="s">
         <v>201</v>
       </c>
-      <c r="K3" t="s">
-        <v>202</v>
-      </c>
-      <c r="L3" t="s">
-        <v>203</v>
-      </c>
-      <c r="M3" t="s">
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A4" s="64">
+        <v>2</v>
+      </c>
+      <c r="B4" s="65" t="s">
+        <v>210</v>
+      </c>
+      <c r="C4" s="66">
+        <v>7</v>
+      </c>
+      <c r="D4" s="108" t="s">
         <v>204</v>
       </c>
-      <c r="N3" t="s">
+      <c r="E4" s="109"/>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A5" s="64">
+        <v>3</v>
+      </c>
+      <c r="B5" s="66">
+        <v>2</v>
+      </c>
+      <c r="C5" s="66">
+        <v>0</v>
+      </c>
+      <c r="D5" s="106" t="s">
         <v>205</v>
       </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A4" s="103">
-        <v>2</v>
-      </c>
-      <c r="B4" s="104" t="s">
-        <v>214</v>
-      </c>
-      <c r="C4" s="105">
+      <c r="E5" s="107"/>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A6" s="64">
+        <v>4</v>
+      </c>
+      <c r="B6" s="66">
+        <v>6</v>
+      </c>
+      <c r="C6" s="66">
+        <v>8</v>
+      </c>
+      <c r="D6" s="105" t="s">
+        <v>206</v>
+      </c>
+      <c r="E6" s="105"/>
+      <c r="K6" s="124" t="s">
+        <v>235</v>
+      </c>
+      <c r="L6" s="102" t="s">
+        <v>243</v>
+      </c>
+      <c r="M6" s="102"/>
+      <c r="N6" s="102"/>
+      <c r="O6" s="102"/>
+      <c r="P6" s="102"/>
+      <c r="Q6" s="102"/>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A7" s="64">
+        <v>5</v>
+      </c>
+      <c r="B7" s="66">
+        <v>8</v>
+      </c>
+      <c r="C7" s="66">
+        <v>6</v>
+      </c>
+      <c r="D7" s="104" t="s">
+        <v>207</v>
+      </c>
+      <c r="E7" s="104"/>
+      <c r="K7" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="L7" s="86"/>
+      <c r="M7" s="86"/>
+      <c r="N7" s="86"/>
+      <c r="O7" s="86"/>
+      <c r="P7" s="86"/>
+      <c r="Q7" s="86"/>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A8" s="64">
+        <v>6</v>
+      </c>
+      <c r="B8" s="66">
+        <v>9</v>
+      </c>
+      <c r="C8" s="66">
+        <v>6</v>
+      </c>
+      <c r="D8" s="103" t="s">
+        <v>208</v>
+      </c>
+      <c r="E8" s="103"/>
+      <c r="K8" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="L8" s="86"/>
+      <c r="M8" s="86"/>
+      <c r="N8" s="86"/>
+      <c r="O8" s="86"/>
+      <c r="P8" s="86"/>
+      <c r="Q8" s="86"/>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A9" s="64">
         <v>7</v>
       </c>
-      <c r="D4" s="108" t="s">
-        <v>208</v>
-      </c>
-      <c r="E4" s="109"/>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A5" s="103">
-        <v>3</v>
-      </c>
-      <c r="B5" s="105">
-        <v>2</v>
-      </c>
-      <c r="C5" s="105">
-        <v>0</v>
-      </c>
-      <c r="D5" s="110" t="s">
+      <c r="B9" s="66">
+        <v>9.01</v>
+      </c>
+      <c r="C9" s="66">
+        <v>7</v>
+      </c>
+      <c r="D9" s="101" t="s">
         <v>209</v>
       </c>
-      <c r="E5" s="111"/>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A6" s="103">
-        <v>4</v>
-      </c>
-      <c r="B6" s="105">
+      <c r="E9" s="101"/>
+      <c r="K9" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="L9" s="86"/>
+      <c r="M9" s="86"/>
+      <c r="N9" s="86"/>
+      <c r="O9" s="86"/>
+      <c r="P9" s="86"/>
+      <c r="Q9" s="86"/>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A10" s="64">
+        <v>8</v>
+      </c>
+      <c r="B10" s="66">
+        <v>-2</v>
+      </c>
+      <c r="C10" s="126">
         <v>6</v>
       </c>
-      <c r="C6" s="105">
-        <v>0</v>
-      </c>
-      <c r="D6" s="112" t="s">
-        <v>210</v>
-      </c>
-      <c r="E6" s="112"/>
-      <c r="K6" s="35" t="s">
-        <v>215</v>
-      </c>
-      <c r="L6" s="35" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A7" s="103">
-        <v>5</v>
-      </c>
-      <c r="B7" s="105">
-        <v>8</v>
-      </c>
-      <c r="C7" s="105">
-        <v>6</v>
-      </c>
-      <c r="D7" s="113" t="s">
-        <v>211</v>
-      </c>
-      <c r="E7" s="113"/>
-      <c r="K7" t="s">
-        <v>216</v>
-      </c>
-      <c r="L7">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A8" s="103">
-        <v>6</v>
-      </c>
-      <c r="B8" s="105">
+      <c r="D10" s="101" t="s">
+        <v>245</v>
+      </c>
+      <c r="E10" s="101"/>
+      <c r="K10" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="L10" s="86"/>
+      <c r="M10" s="86"/>
+      <c r="N10" s="86"/>
+      <c r="O10" s="86"/>
+      <c r="P10" s="86"/>
+      <c r="Q10" s="86"/>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A11" s="64">
         <v>9</v>
       </c>
-      <c r="C8" s="105">
-        <v>6</v>
-      </c>
-      <c r="D8" s="114" t="s">
-        <v>212</v>
-      </c>
-      <c r="E8" s="114"/>
-      <c r="K8" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A9" s="103">
+      <c r="B11" s="66">
+        <v>10</v>
+      </c>
+      <c r="C11" s="126">
         <v>7</v>
       </c>
-      <c r="B9" s="105">
-        <v>9.01</v>
-      </c>
-      <c r="C9" s="105">
-        <v>7</v>
-      </c>
-      <c r="D9" s="107" t="s">
-        <v>213</v>
-      </c>
-      <c r="E9" s="107"/>
-      <c r="K9" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A10" s="103">
-        <v>8</v>
-      </c>
-      <c r="B10" s="105">
-        <v>-2</v>
-      </c>
-      <c r="C10" s="115">
-        <v>6</v>
-      </c>
-      <c r="D10" s="116" t="s">
+      <c r="D11" s="101" t="s">
+        <v>245</v>
+      </c>
+      <c r="E11" s="101"/>
+      <c r="K11" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="L11" s="86"/>
+      <c r="M11" s="86"/>
+      <c r="N11" s="86"/>
+      <c r="O11" s="86"/>
+      <c r="P11" s="86"/>
+      <c r="Q11" s="86"/>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A12" s="64">
+        <v>10</v>
+      </c>
+      <c r="B12" s="66">
+        <v>-1</v>
+      </c>
+      <c r="C12" s="66"/>
+      <c r="D12" s="102" t="s">
         <v>24</v>
       </c>
-      <c r="E10" s="116"/>
-      <c r="K10" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A11" s="103">
-        <v>9</v>
-      </c>
-      <c r="B11" s="105">
-        <v>10</v>
-      </c>
-      <c r="C11" s="115">
-        <v>7</v>
-      </c>
-      <c r="D11" s="116" t="s">
+      <c r="E12" s="102"/>
+      <c r="K12" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="L12" s="86"/>
+      <c r="M12" s="86"/>
+      <c r="N12" s="86"/>
+      <c r="O12" s="86"/>
+      <c r="P12" s="86"/>
+      <c r="Q12" s="86"/>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A13" s="64">
+        <v>11</v>
+      </c>
+      <c r="B13" s="66">
+        <v>0</v>
+      </c>
+      <c r="C13" s="66"/>
+      <c r="D13" s="102" t="s">
         <v>24</v>
       </c>
-      <c r="E11" s="116"/>
-      <c r="K11" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A12" s="103">
-        <v>10</v>
-      </c>
-      <c r="B12" s="105"/>
-      <c r="C12" s="105"/>
-      <c r="D12" s="116" t="s">
+      <c r="E13" s="102"/>
+      <c r="K13" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="L13" s="86"/>
+      <c r="M13" s="86"/>
+      <c r="N13" s="86"/>
+      <c r="O13" s="86"/>
+      <c r="P13" s="86"/>
+      <c r="Q13" s="86"/>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A14" s="64">
+        <v>12</v>
+      </c>
+      <c r="B14" s="66">
+        <v>2.0099999999999998</v>
+      </c>
+      <c r="C14" s="66"/>
+      <c r="D14" s="102" t="s">
         <v>24</v>
       </c>
-      <c r="E12" s="116"/>
-      <c r="K12" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A13" s="103">
-        <v>11</v>
-      </c>
-      <c r="B13" s="105"/>
-      <c r="C13" s="105"/>
-      <c r="D13" s="116" t="s">
+      <c r="E14" s="102"/>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A15" s="64">
+        <v>13</v>
+      </c>
+      <c r="B15" s="66">
+        <v>6.01</v>
+      </c>
+      <c r="C15" s="66"/>
+      <c r="D15" s="102" t="s">
         <v>24</v>
       </c>
-      <c r="E13" s="116"/>
-      <c r="K13" t="s">
-        <v>222</v>
-      </c>
+      <c r="E15" s="102"/>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A16" s="64">
+        <v>14</v>
+      </c>
+      <c r="B16" s="66">
+        <v>8.01</v>
+      </c>
+      <c r="C16" s="66"/>
+      <c r="D16" s="102" t="s">
+        <v>24</v>
+      </c>
+      <c r="E16" s="102"/>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A17" s="64">
+        <v>15</v>
+      </c>
+      <c r="B17" s="66"/>
+      <c r="C17" s="66"/>
+      <c r="D17" s="102"/>
+      <c r="E17" s="102"/>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A18" s="64">
+        <v>16</v>
+      </c>
+      <c r="B18" s="66"/>
+      <c r="C18" s="66"/>
+      <c r="D18" s="102"/>
+      <c r="E18" s="102"/>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A19" s="64">
+        <v>17</v>
+      </c>
+      <c r="B19" s="66"/>
+      <c r="C19" s="66"/>
+      <c r="D19" s="102"/>
+      <c r="E19" s="102"/>
+      <c r="N19" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A20" s="64">
+        <v>18</v>
+      </c>
+      <c r="B20" s="66"/>
+      <c r="C20" s="66"/>
+      <c r="D20" s="102"/>
+      <c r="E20" s="102"/>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A21" s="64">
+        <v>19</v>
+      </c>
+      <c r="B21" s="66"/>
+      <c r="C21" s="66"/>
+      <c r="D21" s="102"/>
+      <c r="E21" s="102"/>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A22" s="64">
+        <v>20</v>
+      </c>
+      <c r="B22" s="66"/>
+      <c r="C22" s="66"/>
+      <c r="D22" s="102"/>
+      <c r="E22" s="102"/>
     </row>
   </sheetData>
-  <mergeCells count="13">
+  <mergeCells count="30">
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="L11:Q11"/>
+    <mergeCell ref="L12:Q12"/>
+    <mergeCell ref="L13:Q13"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="L6:Q6"/>
+    <mergeCell ref="L7:Q7"/>
+    <mergeCell ref="L8:Q8"/>
+    <mergeCell ref="L9:Q9"/>
+    <mergeCell ref="L10:Q10"/>
     <mergeCell ref="D3:E3"/>
     <mergeCell ref="D11:E11"/>
     <mergeCell ref="D12:E12"/>

</xml_diff>